<commit_message>
complete getlast gethist data
</commit_message>
<xml_diff>
--- a/xls/create-test-data.xlsx
+++ b/xls/create-test-data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="24912" windowHeight="12840" activeTab="5"/>
+    <workbookView xWindow="120" yWindow="60" windowWidth="24912" windowHeight="12840" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Корр-каналы" sheetId="5" r:id="rId1"/>
@@ -3496,7 +3496,7 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K3" sqref="K3:K21"/>
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3579,8 +3579,8 @@
         <v>192</v>
       </c>
       <c r="K3" t="str">
-        <f>CONCATENATE("{ ""flid"": ",A3,",""chid"":",B3,", ""p"": ",C3,", ""t"" :",D3,",""dp"": ",E3,", ""q"":",F3,", ""start"":""",H3,""", ""end"":""",I3,""", ""quality"":",J3,"},")</f>
-        <v>{ "flid": 3,"chid":3, "p": 50.2, "t" :30.2,"dp": 1234.56, "q":12223.7, "start":"2020-02-19T12:00", "end":"2020-02-19T13:00", "quality":192},</v>
+        <f>CONCATENATE("{ ""flid"": ",A3,",""chid"":",B3,", ""p"": ",C3,", ""t"" :",D3,",""dp"": ",E3,", ""q"":",F3,", ""start"":""",H3,""", ""lastupdate"":""",I3,""", ""quality"":",J3,"},")</f>
+        <v>{ "flid": 3,"chid":3, "p": 50.2, "t" :30.2,"dp": 1234.56, "q":12223.7, "start":"2020-02-19T12:00", "lastupdate":"2020-02-19T13:00", "quality":192},</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -3613,8 +3613,8 @@
         <v>192</v>
       </c>
       <c r="K4" t="str">
-        <f t="shared" ref="K4:K21" si="0">CONCATENATE("{ ""flid"": ",A4,",""chid"":",B4,", ""p"": ",C4,", ""t"" :",D4,",""dp"": ",E4,", ""q"":",F4,", ""start"":""",H4,""", ""end"":""",I4,""", ""quality"":",J4,"},")</f>
-        <v>{ "flid": 3,"chid":3, "p": 50.3, "t" :30.3,"dp": 1234.57, "q":12223.8, "start":"2020-02-19T13:00", "end":"2020-02-19T14:00", "quality":192},</v>
+        <f t="shared" ref="K4:K21" si="0">CONCATENATE("{ ""flid"": ",A4,",""chid"":",B4,", ""p"": ",C4,", ""t"" :",D4,",""dp"": ",E4,", ""q"":",F4,", ""start"":""",H4,""", ""lastupdate"":""",I4,""", ""quality"":",J4,"},")</f>
+        <v>{ "flid": 3,"chid":3, "p": 50.3, "t" :30.3,"dp": 1234.57, "q":12223.8, "start":"2020-02-19T13:00", "lastupdate":"2020-02-19T14:00", "quality":192},</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -3648,7 +3648,7 @@
       </c>
       <c r="K5" t="str">
         <f t="shared" si="0"/>
-        <v>{ "flid": 3,"chid":3, "p": 50.4, "t" :30.4,"dp": 1234.58, "q":12223.9, "start":"2020-02-19T14:00", "end":"2020-02-19T15:00", "quality":192},</v>
+        <v>{ "flid": 3,"chid":3, "p": 50.4, "t" :30.4,"dp": 1234.58, "q":12223.9, "start":"2020-02-19T14:00", "lastupdate":"2020-02-19T15:00", "quality":192},</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -3682,7 +3682,7 @@
       </c>
       <c r="K6" t="str">
         <f t="shared" si="0"/>
-        <v>{ "flid": 3,"chid":3, "p": 50.5, "t" :30.5,"dp": 1234.59, "q":12223.10, "start":"2020-02-19T15:00", "end":"2020-02-19T16:00", "quality":192},</v>
+        <v>{ "flid": 3,"chid":3, "p": 50.5, "t" :30.5,"dp": 1234.59, "q":12223.10, "start":"2020-02-19T15:00", "lastupdate":"2020-02-19T16:00", "quality":192},</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -3716,7 +3716,7 @@
       </c>
       <c r="K7" t="str">
         <f t="shared" si="0"/>
-        <v>{ "flid": 3,"chid":3, "p": 50.6, "t" :30.6,"dp": 1234.60, "q":12223.11, "start":"2020-02-19T16:00", "end":"2020-02-19T17:00", "quality":192},</v>
+        <v>{ "flid": 3,"chid":3, "p": 50.6, "t" :30.6,"dp": 1234.60, "q":12223.11, "start":"2020-02-19T16:00", "lastupdate":"2020-02-19T17:00", "quality":192},</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -3750,7 +3750,7 @@
       </c>
       <c r="K8" t="str">
         <f t="shared" si="0"/>
-        <v>{ "flid": 3,"chid":3, "p": 50.7, "t" :30.7,"dp": 1234.61, "q":12223.12, "start":"2020-02-19T17:00", "end":"2020-02-19T18:00", "quality":192},</v>
+        <v>{ "flid": 3,"chid":3, "p": 50.7, "t" :30.7,"dp": 1234.61, "q":12223.12, "start":"2020-02-19T17:00", "lastupdate":"2020-02-19T18:00", "quality":192},</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -3784,7 +3784,7 @@
       </c>
       <c r="K9" t="str">
         <f t="shared" si="0"/>
-        <v>{ "flid": 3,"chid":3, "p": 50.8, "t" :30.8,"dp": 1234.62, "q":12223.13, "start":"2020-02-19T18:00", "end":"2020-02-19T19:00", "quality":192},</v>
+        <v>{ "flid": 3,"chid":3, "p": 50.8, "t" :30.8,"dp": 1234.62, "q":12223.13, "start":"2020-02-19T18:00", "lastupdate":"2020-02-19T19:00", "quality":192},</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -3818,7 +3818,7 @@
       </c>
       <c r="K10" t="str">
         <f t="shared" si="0"/>
-        <v>{ "flid": 3,"chid":3, "p": 50.9, "t" :30.9,"dp": 1234.63, "q":12223.14, "start":"2020-02-19T19:00", "end":"2020-02-19T20:00", "quality":192},</v>
+        <v>{ "flid": 3,"chid":3, "p": 50.9, "t" :30.9,"dp": 1234.63, "q":12223.14, "start":"2020-02-19T19:00", "lastupdate":"2020-02-19T20:00", "quality":192},</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -3852,7 +3852,7 @@
       </c>
       <c r="K11" t="str">
         <f t="shared" si="0"/>
-        <v>{ "flid": 3,"chid":3, "p": 50.10, "t" :30.10,"dp": 1234.64, "q":12223.15, "start":"2020-02-19T20:00", "end":"2020-02-19T21:00", "quality":192},</v>
+        <v>{ "flid": 3,"chid":3, "p": 50.10, "t" :30.10,"dp": 1234.64, "q":12223.15, "start":"2020-02-19T20:00", "lastupdate":"2020-02-19T21:00", "quality":192},</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -3886,7 +3886,7 @@
       </c>
       <c r="K12" t="str">
         <f t="shared" si="0"/>
-        <v>{ "flid": 3,"chid":3, "p": 50.11, "t" :30.11,"dp": 1234.65, "q":12223.16, "start":"2020-02-19T21:00", "end":"2020-02-19T22:00", "quality":192},</v>
+        <v>{ "flid": 3,"chid":3, "p": 50.11, "t" :30.11,"dp": 1234.65, "q":12223.16, "start":"2020-02-19T21:00", "lastupdate":"2020-02-19T22:00", "quality":192},</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -3920,7 +3920,7 @@
       </c>
       <c r="K13" t="str">
         <f t="shared" si="0"/>
-        <v>{ "flid": 3,"chid":3, "p": 50.12, "t" :30.12,"dp": 1234.66, "q":12223.17, "start":"2020-02-19T22:00", "end":"2020-02-19T23:00", "quality":192},</v>
+        <v>{ "flid": 3,"chid":3, "p": 50.12, "t" :30.12,"dp": 1234.66, "q":12223.17, "start":"2020-02-19T22:00", "lastupdate":"2020-02-19T23:00", "quality":192},</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -3954,7 +3954,7 @@
       </c>
       <c r="K14" t="str">
         <f t="shared" si="0"/>
-        <v>{ "flid": 3,"chid":3, "p": 50.13, "t" :30.13,"dp": 1234.67, "q":12223.18, "start":"2020-02-19T23:00", "end":"2020-02-19T12:00", "quality":192},</v>
+        <v>{ "flid": 3,"chid":3, "p": 50.13, "t" :30.13,"dp": 1234.67, "q":12223.18, "start":"2020-02-19T23:00", "lastupdate":"2020-02-19T12:00", "quality":192},</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -3988,7 +3988,7 @@
       </c>
       <c r="K15" t="str">
         <f t="shared" si="0"/>
-        <v>{ "flid": 4,"chid":4, "p": 50.14, "t" :30.14,"dp": 1234.68, "q":12223.19, "start":"2020-02-19T12:00", "end":"2020-02-19T13:00", "quality":192},</v>
+        <v>{ "flid": 4,"chid":4, "p": 50.14, "t" :30.14,"dp": 1234.68, "q":12223.19, "start":"2020-02-19T12:00", "lastupdate":"2020-02-19T13:00", "quality":192},</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -4022,7 +4022,7 @@
       </c>
       <c r="K16" t="str">
         <f t="shared" si="0"/>
-        <v>{ "flid": 4,"chid":4, "p": 50.15, "t" :30.15,"dp": 1234.69, "q":12223.20, "start":"2020-02-19T13:00", "end":"2020-02-19T14:00", "quality":192},</v>
+        <v>{ "flid": 4,"chid":4, "p": 50.15, "t" :30.15,"dp": 1234.69, "q":12223.20, "start":"2020-02-19T13:00", "lastupdate":"2020-02-19T14:00", "quality":192},</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
@@ -4056,7 +4056,7 @@
       </c>
       <c r="K17" t="str">
         <f t="shared" si="0"/>
-        <v>{ "flid": 4,"chid":4, "p": 50.16, "t" :30.16,"dp": 1234.70, "q":12223.21, "start":"2020-02-19T14:00", "end":"2020-02-19T15:00", "quality":192},</v>
+        <v>{ "flid": 4,"chid":4, "p": 50.16, "t" :30.16,"dp": 1234.70, "q":12223.21, "start":"2020-02-19T14:00", "lastupdate":"2020-02-19T15:00", "quality":192},</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
@@ -4090,7 +4090,7 @@
       </c>
       <c r="K18" t="str">
         <f t="shared" si="0"/>
-        <v>{ "flid": 4,"chid":4, "p": 50.17, "t" :30.17,"dp": 1234.71, "q":12223.22, "start":"2020-02-19T15:00", "end":"2020-02-19T16:00", "quality":192},</v>
+        <v>{ "flid": 4,"chid":4, "p": 50.17, "t" :30.17,"dp": 1234.71, "q":12223.22, "start":"2020-02-19T15:00", "lastupdate":"2020-02-19T16:00", "quality":192},</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
@@ -4124,7 +4124,7 @@
       </c>
       <c r="K19" t="str">
         <f t="shared" si="0"/>
-        <v>{ "flid": 4,"chid":4, "p": 50.18, "t" :30.18,"dp": 1234.72, "q":12223.23, "start":"2020-02-19T16:00", "end":"2020-02-19T17:00", "quality":192},</v>
+        <v>{ "flid": 4,"chid":4, "p": 50.18, "t" :30.18,"dp": 1234.72, "q":12223.23, "start":"2020-02-19T16:00", "lastupdate":"2020-02-19T17:00", "quality":192},</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
@@ -4158,7 +4158,7 @@
       </c>
       <c r="K20" t="str">
         <f t="shared" si="0"/>
-        <v>{ "flid": 4,"chid":4, "p": 50.19, "t" :30.19,"dp": 1234.73, "q":12223.24, "start":"2020-02-19T17:00", "end":"2020-02-19T18:00", "quality":192},</v>
+        <v>{ "flid": 4,"chid":4, "p": 50.19, "t" :30.19,"dp": 1234.73, "q":12223.24, "start":"2020-02-19T17:00", "lastupdate":"2020-02-19T18:00", "quality":192},</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
@@ -4192,7 +4192,7 @@
       </c>
       <c r="K21" t="str">
         <f t="shared" si="0"/>
-        <v>{ "flid": 4,"chid":4, "p": 50.20, "t" :30.20,"dp": 1234.74, "q":12223.25, "start":"2020-02-19T18:00", "end":"2020-02-19T19:00", "quality":192},</v>
+        <v>{ "flid": 4,"chid":4, "p": 50.20, "t" :30.20,"dp": 1234.74, "q":12223.25, "start":"2020-02-19T18:00", "lastupdate":"2020-02-19T19:00", "quality":192},</v>
       </c>
     </row>
   </sheetData>
@@ -4204,8 +4204,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4284,8 +4284,8 @@
         <v>192</v>
       </c>
       <c r="K3" t="str">
-        <f>CONCATENATE("{ ""flid"": ",A3,",""chid"":",B3,", ""p"": ",C3,", ""t"" :",D3,",""dp"": ",E3,", ""q"":",F3,", ""start"":""",H3,""", ""end"":""",I3,""", ""quality"":",J3,"},")</f>
-        <v>{ "flid": 3,"chid":3, "p": 50.2, "t" :30.2,"dp": 1234.56, "q":122523.7, "start":"2020-02-01T07:00", "end":"2020-02-02T07:00", "quality":192},</v>
+        <f>CONCATENATE("{ ""flid"": ",A3,",""chid"":",B3,", ""p"": ",C3,", ""t"" :",D3,",""dp"": ",E3,", ""q"":",F3,", ""start"":""",H3,""", ""lastupdate"":""",I3,""", ""quality"":",J3,"},")</f>
+        <v>{ "flid": 3,"chid":3, "p": 50.2, "t" :30.2,"dp": 1234.56, "q":122523.7, "start":"2020-02-01T07:00", "lastupdate":"2020-02-02T07:00", "quality":192},</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -4318,8 +4318,8 @@
         <v>192</v>
       </c>
       <c r="K4" t="str">
-        <f t="shared" ref="K4:K21" si="0">CONCATENATE("{ ""flid"": ",A4,",""chid"":",B4,", ""p"": ",C4,", ""t"" :",D4,",""dp"": ",E4,", ""q"":",F4,", ""start"":""",H4,""", ""end"":""",I4,""", ""quality"":",J4,"},")</f>
-        <v>{ "flid": 3,"chid":3, "p": 50.3, "t" :30.3,"dp": 1234.57, "q":122523.8, "start":"2020-02-02T07:00", "end":"2020-02-03T07:00", "quality":192},</v>
+        <f t="shared" ref="K4:K21" si="0">CONCATENATE("{ ""flid"": ",A4,",""chid"":",B4,", ""p"": ",C4,", ""t"" :",D4,",""dp"": ",E4,", ""q"":",F4,", ""start"":""",H4,""", ""lastupdate"":""",I4,""", ""quality"":",J4,"},")</f>
+        <v>{ "flid": 3,"chid":3, "p": 50.3, "t" :30.3,"dp": 1234.57, "q":122523.8, "start":"2020-02-02T07:00", "lastupdate":"2020-02-03T07:00", "quality":192},</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -4353,7 +4353,7 @@
       </c>
       <c r="K5" t="str">
         <f t="shared" si="0"/>
-        <v>{ "flid": 3,"chid":3, "p": 50.4, "t" :30.4,"dp": 1234.58, "q":122523.9, "start":"2020-02-03T07:00", "end":"2020-02-04T07:00", "quality":192},</v>
+        <v>{ "flid": 3,"chid":3, "p": 50.4, "t" :30.4,"dp": 1234.58, "q":122523.9, "start":"2020-02-03T07:00", "lastupdate":"2020-02-04T07:00", "quality":192},</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -4387,7 +4387,7 @@
       </c>
       <c r="K6" t="str">
         <f t="shared" si="0"/>
-        <v>{ "flid": 3,"chid":3, "p": 50.5, "t" :30.5,"dp": 1234.59, "q":122523.10, "start":"2020-02-04T07:00", "end":"2020-02-05T07:00", "quality":192},</v>
+        <v>{ "flid": 3,"chid":3, "p": 50.5, "t" :30.5,"dp": 1234.59, "q":122523.10, "start":"2020-02-04T07:00", "lastupdate":"2020-02-05T07:00", "quality":192},</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -4421,7 +4421,7 @@
       </c>
       <c r="K7" t="str">
         <f t="shared" si="0"/>
-        <v>{ "flid": 3,"chid":3, "p": 50.6, "t" :30.6,"dp": 1234.60, "q":122523.11, "start":"2020-02-05T07:00", "end":"2020-02-06T07:00", "quality":192},</v>
+        <v>{ "flid": 3,"chid":3, "p": 50.6, "t" :30.6,"dp": 1234.60, "q":122523.11, "start":"2020-02-05T07:00", "lastupdate":"2020-02-06T07:00", "quality":192},</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -4455,7 +4455,7 @@
       </c>
       <c r="K8" t="str">
         <f t="shared" si="0"/>
-        <v>{ "flid": 3,"chid":3, "p": 50.7, "t" :30.7,"dp": 1234.61, "q":122523.12, "start":"2020-02-06T07:00", "end":"2020-02-07T07:00", "quality":192},</v>
+        <v>{ "flid": 3,"chid":3, "p": 50.7, "t" :30.7,"dp": 1234.61, "q":122523.12, "start":"2020-02-06T07:00", "lastupdate":"2020-02-07T07:00", "quality":192},</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -4489,7 +4489,7 @@
       </c>
       <c r="K9" t="str">
         <f t="shared" si="0"/>
-        <v>{ "flid": 3,"chid":3, "p": 50.8, "t" :30.8,"dp": 1234.62, "q":122523.13, "start":"2020-02-07T07:00", "end":"2020-02-08T07:00", "quality":192},</v>
+        <v>{ "flid": 3,"chid":3, "p": 50.8, "t" :30.8,"dp": 1234.62, "q":122523.13, "start":"2020-02-07T07:00", "lastupdate":"2020-02-08T07:00", "quality":192},</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -4523,7 +4523,7 @@
       </c>
       <c r="K10" t="str">
         <f t="shared" si="0"/>
-        <v>{ "flid": 3,"chid":3, "p": 50.9, "t" :30.9,"dp": 1234.63, "q":122523.14, "start":"2020-02-08T07:00", "end":"2020-02-09T07:00", "quality":192},</v>
+        <v>{ "flid": 3,"chid":3, "p": 50.9, "t" :30.9,"dp": 1234.63, "q":122523.14, "start":"2020-02-08T07:00", "lastupdate":"2020-02-09T07:00", "quality":192},</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -4557,7 +4557,7 @@
       </c>
       <c r="K11" t="str">
         <f t="shared" si="0"/>
-        <v>{ "flid": 3,"chid":3, "p": 50.10, "t" :30.10,"dp": 1234.64, "q":122523.15, "start":"2020-02-09T07:00", "end":"2020-02-10T07:00", "quality":192},</v>
+        <v>{ "flid": 3,"chid":3, "p": 50.10, "t" :30.10,"dp": 1234.64, "q":122523.15, "start":"2020-02-09T07:00", "lastupdate":"2020-02-10T07:00", "quality":192},</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -4591,7 +4591,7 @@
       </c>
       <c r="K12" t="str">
         <f t="shared" si="0"/>
-        <v>{ "flid": 4,"chid":4, "p": 50.11, "t" :30.11,"dp": 1234.65, "q":122523.16, "start":"2020-02-01T07:00", "end":"2020-02-02T07:00", "quality":192},</v>
+        <v>{ "flid": 4,"chid":4, "p": 50.11, "t" :30.11,"dp": 1234.65, "q":122523.16, "start":"2020-02-01T07:00", "lastupdate":"2020-02-02T07:00", "quality":192},</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -4625,7 +4625,7 @@
       </c>
       <c r="K13" t="str">
         <f t="shared" si="0"/>
-        <v>{ "flid": 4,"chid":4, "p": 50.12, "t" :30.12,"dp": 1234.66, "q":122523.17, "start":"2020-02-02T07:00", "end":"2020-02-03T07:00", "quality":192},</v>
+        <v>{ "flid": 4,"chid":4, "p": 50.12, "t" :30.12,"dp": 1234.66, "q":122523.17, "start":"2020-02-02T07:00", "lastupdate":"2020-02-03T07:00", "quality":192},</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -4659,7 +4659,7 @@
       </c>
       <c r="K14" t="str">
         <f t="shared" si="0"/>
-        <v>{ "flid": 4,"chid":4, "p": 50.13, "t" :30.13,"dp": 1234.67, "q":122523.18, "start":"2020-02-03T07:00", "end":"2020-02-04T07:00", "quality":192},</v>
+        <v>{ "flid": 4,"chid":4, "p": 50.13, "t" :30.13,"dp": 1234.67, "q":122523.18, "start":"2020-02-03T07:00", "lastupdate":"2020-02-04T07:00", "quality":192},</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -4693,7 +4693,7 @@
       </c>
       <c r="K15" t="str">
         <f t="shared" si="0"/>
-        <v>{ "flid": 4,"chid":4, "p": 50.14, "t" :30.14,"dp": 1234.68, "q":122523.19, "start":"2020-02-04T07:00", "end":"2020-02-05T07:00", "quality":192},</v>
+        <v>{ "flid": 4,"chid":4, "p": 50.14, "t" :30.14,"dp": 1234.68, "q":122523.19, "start":"2020-02-04T07:00", "lastupdate":"2020-02-05T07:00", "quality":192},</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -4727,7 +4727,7 @@
       </c>
       <c r="K16" t="str">
         <f t="shared" si="0"/>
-        <v>{ "flid": 4,"chid":4, "p": 50.15, "t" :30.15,"dp": 1234.69, "q":122523.20, "start":"2020-02-05T07:00", "end":"2020-02-06T07:00", "quality":192},</v>
+        <v>{ "flid": 4,"chid":4, "p": 50.15, "t" :30.15,"dp": 1234.69, "q":122523.20, "start":"2020-02-05T07:00", "lastupdate":"2020-02-06T07:00", "quality":192},</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
@@ -4761,7 +4761,7 @@
       </c>
       <c r="K17" t="str">
         <f t="shared" si="0"/>
-        <v>{ "flid": 4,"chid":4, "p": 50.16, "t" :30.16,"dp": 1234.70, "q":122523.21, "start":"2020-02-06T07:00", "end":"2020-02-07T07:00", "quality":192},</v>
+        <v>{ "flid": 4,"chid":4, "p": 50.16, "t" :30.16,"dp": 1234.70, "q":122523.21, "start":"2020-02-06T07:00", "lastupdate":"2020-02-07T07:00", "quality":192},</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
@@ -4795,7 +4795,7 @@
       </c>
       <c r="K18" t="str">
         <f t="shared" si="0"/>
-        <v>{ "flid": 4,"chid":4, "p": 50.17, "t" :30.17,"dp": 1234.71, "q":122523.22, "start":"2020-02-07T07:00", "end":"2020-02-08T07:00", "quality":192},</v>
+        <v>{ "flid": 4,"chid":4, "p": 50.17, "t" :30.17,"dp": 1234.71, "q":122523.22, "start":"2020-02-07T07:00", "lastupdate":"2020-02-08T07:00", "quality":192},</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
@@ -4829,7 +4829,7 @@
       </c>
       <c r="K19" t="str">
         <f t="shared" si="0"/>
-        <v>{ "flid": 4,"chid":4, "p": 50.18, "t" :30.18,"dp": 1234.72, "q":122523.23, "start":"2020-02-08T07:00", "end":"2020-02-09T07:00", "quality":192},</v>
+        <v>{ "flid": 4,"chid":4, "p": 50.18, "t" :30.18,"dp": 1234.72, "q":122523.23, "start":"2020-02-08T07:00", "lastupdate":"2020-02-09T07:00", "quality":192},</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
@@ -4863,7 +4863,7 @@
       </c>
       <c r="K20" t="str">
         <f t="shared" si="0"/>
-        <v>{ "flid": 4,"chid":4, "p": 50.19, "t" :30.19,"dp": 1234.73, "q":122523.24, "start":"2020-02-09T07:00", "end":"2020-02-10T07:00", "quality":192},</v>
+        <v>{ "flid": 4,"chid":4, "p": 50.19, "t" :30.19,"dp": 1234.73, "q":122523.24, "start":"2020-02-09T07:00", "lastupdate":"2020-02-10T07:00", "quality":192},</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
@@ -4897,7 +4897,7 @@
       </c>
       <c r="K21" t="str">
         <f t="shared" si="0"/>
-        <v>{ "flid": 4,"chid":4, "p": 50.20, "t" :30.20,"dp": 1234.74, "q":122523.25, "start":"2020-02-10T07:00", "end":"2020-02-11T07:00", "quality":192},</v>
+        <v>{ "flid": 4,"chid":4, "p": 50.20, "t" :30.20,"dp": 1234.74, "q":122523.25, "start":"2020-02-10T07:00", "lastupdate":"2020-02-11T07:00", "quality":192},</v>
       </c>
     </row>
   </sheetData>
@@ -4910,7 +4910,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
generic repo & controll
</commit_message>
<xml_diff>
--- a/xls/create-test-data.xlsx
+++ b/xls/create-test-data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="24915" windowHeight="12840" activeTab="7"/>
+    <workbookView xWindow="120" yWindow="60" windowWidth="24915" windowHeight="12840" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Корр-каналы" sheetId="5" r:id="rId1"/>
@@ -15,13 +15,14 @@
     <sheet name="StatHlData" sheetId="8" r:id="rId6"/>
     <sheet name="rtsystem" sheetId="9" r:id="rId7"/>
     <sheet name="rtdata" sheetId="10" r:id="rId8"/>
+    <sheet name="regimParam" sheetId="11" r:id="rId9"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="833" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="879" uniqueCount="220">
   <si>
     <t>isAbsP</t>
   </si>
@@ -609,6 +610,78 @@
   </si>
   <si>
     <t>good</t>
+  </si>
+  <si>
+    <t>P in KC-1</t>
+  </si>
+  <si>
+    <t>P in KC-2</t>
+  </si>
+  <si>
+    <t>P in KC-3</t>
+  </si>
+  <si>
+    <t>P in KC-4</t>
+  </si>
+  <si>
+    <t>P in KC-5</t>
+  </si>
+  <si>
+    <t>P in KC-6</t>
+  </si>
+  <si>
+    <t>P in KC-7</t>
+  </si>
+  <si>
+    <t>P in KC-8</t>
+  </si>
+  <si>
+    <t>P in KC-9</t>
+  </si>
+  <si>
+    <t>P in KC-10</t>
+  </si>
+  <si>
+    <t>P in KC-11</t>
+  </si>
+  <si>
+    <t>P in KC-12</t>
+  </si>
+  <si>
+    <t>P in KC-13</t>
+  </si>
+  <si>
+    <t>P in KC-14</t>
+  </si>
+  <si>
+    <t>P in KC-15</t>
+  </si>
+  <si>
+    <t>P in KC-16</t>
+  </si>
+  <si>
+    <t>P in KC-17</t>
+  </si>
+  <si>
+    <t>P in KC-18</t>
+  </si>
+  <si>
+    <t>P in KC-19</t>
+  </si>
+  <si>
+    <t>P in KC-20</t>
+  </si>
+  <si>
+    <t>P in KC-21</t>
+  </si>
+  <si>
+    <t>P in KC-22</t>
+  </si>
+  <si>
+    <t>P in KC-23</t>
+  </si>
+  <si>
+    <t>P in KC-24</t>
   </si>
 </sst>
 </file>
@@ -3431,7 +3504,7 @@
         <v>192</v>
       </c>
       <c r="J23" t="str">
-        <f t="shared" ref="J23:J40" si="1">CONCATENATE("{ ""flid"": ",A23,",""chid"":",B23,", ""p"": ",C23,", ""t"" :",D23,",""dp"": ",E23,", ""q"":",F23,", ""currday"":",G23,", ""lastupdate"":""",H23,""", ""quality"":",I23,"},")</f>
+        <f t="shared" ref="J23:J38" si="1">CONCATENATE("{ ""flid"": ",A23,",""chid"":",B23,", ""p"": ",C23,", ""t"" :",D23,",""dp"": ",E23,", ""q"":",F23,", ""currday"":",G23,", ""lastupdate"":""",H23,""", ""quality"":",I23,"},")</f>
         <v>{ "flid": 3,"chid":3, "p": 50, "t" :30,"dp": 1000, "q":100, "currday":1000, "lastupdate":"2020-02-19T12:02", "quality":192},</v>
       </c>
     </row>
@@ -4692,7 +4765,7 @@
         <v>193</v>
       </c>
       <c r="K22" s="51" t="str">
-        <f t="shared" ref="K22:K39" si="1">CONCATENATE("{ ""flid"": ",A22,",""chid"":",B22,", ""p"": ",C22,", ""t"" :",D22,",""dp"": ",E22,", ""q"":",F22,", ""start"":""",H22,""", ""lastupdate"":""",I22,""", ""quality"":",J22,"},")</f>
+        <f t="shared" ref="K22:K38" si="1">CONCATENATE("{ ""flid"": ",A22,",""chid"":",B22,", ""p"": ",C22,", ""t"" :",D22,",""dp"": ",E22,", ""q"":",F22,", ""start"":""",H22,""", ""lastupdate"":""",I22,""", ""quality"":",J22,"},")</f>
         <v>{ "flid": 3,"chid":3, "p": 50, "t" :30,"dp": 1000, "q":100, "start":"2020-02-19T13:00", "lastupdate":"2020-02-19T14:00", "quality":193},</v>
       </c>
     </row>
@@ -8448,8 +8521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J30" sqref="J30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9299,4 +9372,397 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:D26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="49.5703125" customWidth="1"/>
+    <col min="4" max="4" width="42.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="C2" s="45" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="D3" t="str">
+        <f>CONCATENATE("{ ""paramid"": ",A3,",""sensorid"":",B3,", ""name"": """,C3,"""},")</f>
+        <v>{ "paramid": 1,"sensorid":1, "name": "P in KC-1"},</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" ref="D4:D26" si="0">CONCATENATE("{ ""paramid"": ",A4,",""sensorid"":",B4,", ""name"": """,C4,"""},")</f>
+        <v>{ "paramid": 2,"sensorid":2, "name": "P in KC-2"},</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "paramid": 3,"sensorid":3, "name": "P in KC-3"},</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "paramid": 4,"sensorid":4, "name": "P in KC-4"},</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1">
+        <v>5</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "paramid": 5,"sensorid":5, "name": "P in KC-5"},</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1">
+        <v>6</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "paramid": 6,"sensorid":6, "name": "P in KC-6"},</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "paramid": 7,"sensorid":null, "name": "P in KC-7"},</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "paramid": 8,"sensorid":null, "name": "P in KC-8"},</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "paramid": 9,"sensorid":null, "name": "P in KC-9"},</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "paramid": 10,"sensorid":null, "name": "P in KC-10"},</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "paramid": 11,"sensorid":null, "name": "P in KC-11"},</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "paramid": 12,"sensorid":null, "name": "P in KC-12"},</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "paramid": 13,"sensorid":null, "name": "P in KC-13"},</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "paramid": 14,"sensorid":null, "name": "P in KC-14"},</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "paramid": 15,"sensorid":null, "name": "P in KC-15"},</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "paramid": 16,"sensorid":null, "name": "P in KC-16"},</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "paramid": 17,"sensorid":null, "name": "P in KC-17"},</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "paramid": 18,"sensorid":null, "name": "P in KC-18"},</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="D21" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "paramid": 19,"sensorid":null, "name": "P in KC-19"},</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>20</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="D22" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "paramid": 20,"sensorid":null, "name": "P in KC-20"},</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>21</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="D23" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "paramid": 21,"sensorid":null, "name": "P in KC-21"},</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>22</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="D24" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "paramid": 22,"sensorid":null, "name": "P in KC-22"},</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>23</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="D25" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "paramid": 23,"sensorid":null, "name": "P in KC-23"},</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>24</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="D26" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "paramid": 24,"sensorid":null, "name": "P in KC-24"},</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fix generic repo select
</commit_message>
<xml_diff>
--- a/xls/create-test-data.xlsx
+++ b/xls/create-test-data.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\source\node\oask-gtp-webapi\xls\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="24915" windowHeight="12840" activeTab="9"/>
+    <workbookView xWindow="120" yWindow="60" windowWidth="24912" windowHeight="12840" firstSheet="2" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Корр-каналы" sheetId="5" r:id="rId1"/>
@@ -19,12 +24,12 @@
     <sheet name="Forms" sheetId="12" r:id="rId10"/>
     <sheet name="TablesGui" sheetId="13" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1093" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1093" uniqueCount="283">
   <si>
     <t>isAbsP</t>
   </si>
@@ -705,24 +710,6 @@
   </si>
   <si>
     <t>key</t>
-  </si>
-  <si>
-    <t>field1</t>
-  </si>
-  <si>
-    <t>field2</t>
-  </si>
-  <si>
-    <t>field3</t>
-  </si>
-  <si>
-    <t>field5</t>
-  </si>
-  <si>
-    <t>field6</t>
-  </si>
-  <si>
-    <t>field7</t>
   </si>
   <si>
     <t>{"key":"</t>
@@ -896,7 +883,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1378,7 +1365,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1413,7 +1400,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1628,40 +1615,40 @@
       <selection sqref="A1:XFD9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.5546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="108.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.140625" customWidth="1"/>
-    <col min="14" max="14" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="28" max="29" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="101.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="108.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.109375" customWidth="1"/>
+    <col min="14" max="14" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="101.88671875" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="7" customFormat="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:30" s="7" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>32</v>
       </c>
@@ -1745,7 +1732,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:30" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:30" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
         <v>37</v>
       </c>
@@ -1805,7 +1792,7 @@
         <v>{"corrid":1,"name":"Корректор № 1","ip":"192.168.0.111","ftpDir":"./","addr":1,"channels":[</v>
       </c>
     </row>
-    <row r="3" spans="1:30" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="15"/>
       <c r="B3" s="16"/>
       <c r="C3" s="16"/>
@@ -1877,7 +1864,7 @@
         <v>{"chid":1,"chno":1,"name":"Line 1","template":"S001R1","isAbsP":true,"chour":true,"hasR":true,"hasH":true},</v>
       </c>
     </row>
-    <row r="4" spans="1:30" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="15"/>
       <c r="B4" s="16"/>
       <c r="C4" s="16"/>
@@ -1949,7 +1936,7 @@
         <v>{"chid":2,"chno":2,"name":"Line 2","template":"S001R2","isAbsP":true,"chour":true,"hasR":true,"hasH":true},</v>
       </c>
     </row>
-    <row r="5" spans="1:30" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="17"/>
       <c r="B5" s="18"/>
       <c r="C5" s="18"/>
@@ -2021,7 +2008,7 @@
         <v>{"chid":3,"chno":3,"name":"Line 3","template":"S001R3","isAbsP":true,"chour":true,"hasR":true,"hasH":true}]},</v>
       </c>
     </row>
-    <row r="6" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="12" t="s">
         <v>37</v>
       </c>
@@ -2081,7 +2068,7 @@
         <v>{"corrid":2,"name":"Корректор № 2","ip":"192.168.0.112","ftpDir":"./","addr":2,"channels":[</v>
       </c>
     </row>
-    <row r="7" spans="1:30" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="15"/>
       <c r="B7" s="16"/>
       <c r="C7" s="16"/>
@@ -2153,7 +2140,7 @@
         <v>{"chid":4,"chno":1,"name":"Line 1","template":"S001R1","isAbsP":true,"chour":true,"hasR":true,"hasH":true},</v>
       </c>
     </row>
-    <row r="8" spans="1:30" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="15"/>
       <c r="B8" s="16"/>
       <c r="C8" s="16"/>
@@ -2225,7 +2212,7 @@
         <v>{"chid":5,"chno":2,"name":"Line 2","template":"S001R2","isAbsP":true,"chour":true,"hasR":true,"hasH":true},</v>
       </c>
     </row>
-    <row r="9" spans="1:30" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="17"/>
       <c r="B9" s="18"/>
       <c r="C9" s="18"/>
@@ -2297,7 +2284,7 @@
         <v>{"chid":6,"chno":3,"name":"Line 3","template":"S001R3","isAbsP":true,"chour":true,"hasR":true,"hasH":true}]},</v>
       </c>
     </row>
-    <row r="10" spans="1:30" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.3">
       <c r="AD10" s="6" t="s">
         <v>12</v>
       </c>
@@ -2313,32 +2300,32 @@
   <dimension ref="A1:X9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X2" sqref="X2:X9"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="55.140625" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.7109375" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.7109375" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.7109375" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.42578125" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.7109375" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="26.85546875" customWidth="1"/>
+    <col min="6" max="6" width="55.109375" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.6640625" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.6640625" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.44140625" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.6640625" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="26.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" s="7" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>220</v>
       </c>
@@ -2360,34 +2347,34 @@
         <v>226</v>
       </c>
       <c r="I1" s="21" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="J1" s="21" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="K1" s="21" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="L1" s="21" t="s">
         <v>190</v>
       </c>
       <c r="M1" s="21" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="N1" s="21" t="s">
+        <v>240</v>
+      </c>
+      <c r="O1" s="21" t="s">
+        <v>243</v>
+      </c>
+      <c r="P1" s="21" t="s">
+        <v>244</v>
+      </c>
+      <c r="Q1" s="21" t="s">
         <v>246</v>
       </c>
-      <c r="O1" s="21" t="s">
-        <v>249</v>
-      </c>
-      <c r="P1" s="21" t="s">
-        <v>250</v>
-      </c>
-      <c r="Q1" s="21" t="s">
-        <v>252</v>
-      </c>
       <c r="R1" s="21" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="S1" s="21"/>
       <c r="T1" s="21"/>
@@ -2398,7 +2385,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:24" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
         <v>222</v>
       </c>
@@ -2412,7 +2399,7 @@
         <v>223</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="F2" s="13" t="str">
         <f>CONCATENATE(A2,B2,C2,D2,E2)</f>
@@ -2440,7 +2427,7 @@
         <v>{"formid":1,"name":"Форма ввод № 1","controls":[</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="15"/>
       <c r="B3" s="16"/>
       <c r="C3" s="16"/>
@@ -2451,40 +2438,40 @@
         <v/>
       </c>
       <c r="G3" s="8" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>227</v>
+        <v>259</v>
       </c>
       <c r="I3" s="8" t="s">
+        <v>236</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="L3" s="8">
+        <v>100</v>
+      </c>
+      <c r="M3" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="N3" s="8" t="s">
         <v>242</v>
       </c>
-      <c r="J3" s="8" t="s">
-        <v>236</v>
-      </c>
-      <c r="K3" s="8" t="s">
-        <v>244</v>
-      </c>
-      <c r="L3" s="8">
-        <v>100</v>
-      </c>
-      <c r="M3" s="8" t="s">
-        <v>247</v>
-      </c>
-      <c r="N3" s="8" t="s">
-        <v>248</v>
-      </c>
       <c r="O3" s="8" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="P3" s="8">
         <v>1</v>
       </c>
       <c r="Q3" s="8" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="R3" s="8" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="S3" s="8"/>
       <c r="T3" s="8"/>
@@ -2495,10 +2482,10 @@
       </c>
       <c r="X3" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>{"key":"field1","label":"Параметр 1","value":"100","controlType":"textbox","order":1,"options":[{}]},</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>{"key":"param1","label":"Параметр 1","value":"100","controlType":"textbox","order":1,"options":[{}]},</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="15"/>
       <c r="B4" s="16"/>
       <c r="C4" s="16"/>
@@ -2509,40 +2496,40 @@
         <v/>
       </c>
       <c r="G4" s="8" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>228</v>
+        <v>260</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="L4" s="8">
         <v>101</v>
       </c>
       <c r="M4" s="8" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="N4" s="8" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="O4" s="8" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="P4" s="8">
         <v>2</v>
       </c>
       <c r="Q4" s="8" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="R4" s="8" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="S4" s="8"/>
       <c r="T4" s="8"/>
@@ -2553,10 +2540,10 @@
       </c>
       <c r="X4" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>{"key":"field2","label":"Параметр 2","value":"101","controlType":"textbox","order":2,"options":[{}]},</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>{"key":"param2","label":"Параметр 2","value":"101","controlType":"textbox","order":2,"options":[{}]},</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="17"/>
       <c r="B5" s="18"/>
       <c r="C5" s="18"/>
@@ -2567,40 +2554,40 @@
         <v/>
       </c>
       <c r="G5" s="8" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>229</v>
+        <v>261</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="J5" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="K5" s="8" t="s">
         <v>238</v>
-      </c>
-      <c r="K5" s="8" t="s">
-        <v>244</v>
       </c>
       <c r="L5" s="8">
         <v>102</v>
       </c>
       <c r="M5" s="19" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="N5" s="8" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="O5" s="19" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="P5" s="8">
         <v>3</v>
       </c>
       <c r="Q5" s="19" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="R5" s="8" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="S5" s="19"/>
       <c r="T5" s="19"/>
@@ -2611,10 +2598,10 @@
       </c>
       <c r="X5" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>{"key":"field3","label":"Параметр 3","value":"102","controlType":"textbox","order":3,"options":[{}]}]},</v>
-      </c>
-    </row>
-    <row r="6" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>{"key":"param3","label":"Параметр 3","value":"102","controlType":"textbox","order":3,"options":[{}]}]},</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="12" t="s">
         <v>222</v>
       </c>
@@ -2628,7 +2615,7 @@
         <v>224</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="F6" s="13" t="str">
         <f t="shared" si="1"/>
@@ -2656,7 +2643,7 @@
         <v>{"formid":2,"name":"Форма ввод № 2","controls":[</v>
       </c>
     </row>
-    <row r="7" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="15"/>
       <c r="B7" s="16"/>
       <c r="C7" s="16"/>
@@ -2667,40 +2654,40 @@
         <v/>
       </c>
       <c r="G7" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>262</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>236</v>
+      </c>
+      <c r="J7" s="8" t="s">
         <v>233</v>
       </c>
-      <c r="H7" s="8" t="s">
-        <v>230</v>
-      </c>
-      <c r="I7" s="8" t="s">
-        <v>242</v>
-      </c>
-      <c r="J7" s="8" t="s">
-        <v>239</v>
-      </c>
       <c r="K7" s="8" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="L7" s="8">
         <v>104</v>
       </c>
       <c r="M7" s="8" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="N7" s="8" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="O7" s="8" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="P7" s="8">
         <v>5</v>
       </c>
       <c r="Q7" s="8" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="R7" s="8" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="S7" s="8"/>
       <c r="T7" s="8"/>
@@ -2711,10 +2698,10 @@
       </c>
       <c r="X7" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>{"key":"field5","label":"Параметр 5","value":"104","controlType":"textbox","order":5,"options":[{}]},</v>
-      </c>
-    </row>
-    <row r="8" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>{"key":"param5","label":"Параметр 5","value":"104","controlType":"textbox","order":5,"options":[{}]},</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="15"/>
       <c r="B8" s="16"/>
       <c r="C8" s="16"/>
@@ -2725,40 +2712,40 @@
         <v/>
       </c>
       <c r="G8" s="8" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>231</v>
+        <v>263</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="J8" s="8" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="K8" s="8" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="L8" s="8">
         <v>105</v>
       </c>
       <c r="M8" s="8" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="N8" s="8" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="O8" s="8" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="P8" s="8">
         <v>6</v>
       </c>
       <c r="Q8" s="8" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="R8" s="8" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="S8" s="8"/>
       <c r="T8" s="8"/>
@@ -2769,10 +2756,10 @@
       </c>
       <c r="X8" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>{"key":"field6","label":"Параметр 6","value":"105","controlType":"textbox","order":6,"options":[{}]},</v>
-      </c>
-    </row>
-    <row r="9" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>{"key":"param6","label":"Параметр 6","value":"105","controlType":"textbox","order":6,"options":[{}]},</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="17"/>
       <c r="B9" s="18"/>
       <c r="C9" s="18"/>
@@ -2783,40 +2770,40 @@
         <v/>
       </c>
       <c r="G9" s="8" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>232</v>
+        <v>264</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="J9" s="8" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="K9" s="8" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="L9" s="8">
         <v>106</v>
       </c>
       <c r="M9" s="19" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="N9" s="8" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="O9" s="19" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="P9" s="8">
         <v>7</v>
       </c>
       <c r="Q9" s="19" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="R9" s="8" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="S9" s="19"/>
       <c r="T9" s="19"/>
@@ -2827,7 +2814,7 @@
       </c>
       <c r="X9" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>{"key":"field7","label":"Параметр 7","value":"106","controlType":"textbox","order":7,"options":[{}]}]},</v>
+        <v>{"key":"param7","label":"Параметр 7","value":"106","controlType":"textbox","order":7,"options":[{}]}]},</v>
       </c>
     </row>
   </sheetData>
@@ -2840,39 +2827,39 @@
   <dimension ref="A1:X21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="X2" sqref="X2:X21"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="23.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="23.6640625" customWidth="1"/>
     <col min="5" max="5" width="16" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="56.28515625" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="56.33203125" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.85546875" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="20.7109375" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="13.7109375" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="12.42578125" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="6.7109375" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="13.7109375" hidden="1" customWidth="1"/>
+    <col min="10" max="11" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.88671875" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="20.6640625" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="13.6640625" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="12.44140625" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="6.6640625" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="13.6640625" hidden="1" customWidth="1"/>
     <col min="18" max="18" width="9" hidden="1" customWidth="1"/>
     <col min="19" max="22" width="0" hidden="1" customWidth="1"/>
-    <col min="23" max="23" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="96.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="96.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" s="7" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="C1" s="11" t="s">
         <v>33</v>
@@ -2889,10 +2876,10 @@
         <v>3</v>
       </c>
       <c r="I1" s="21" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="J1" s="21" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="K1" s="21"/>
       <c r="L1" s="21"/>
@@ -2911,9 +2898,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:24" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="B2" s="13">
         <v>1</v>
@@ -2922,10 +2909,10 @@
         <v>43</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="F2" s="13" t="str">
         <f>CONCATENATE(A2,B2,C2,D2,E2)</f>
@@ -2953,7 +2940,7 @@
         <v>{"tableid":1,"name":"Таблица ввод № 1","columns":[</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="15"/>
       <c r="B3" s="16"/>
       <c r="C3" s="16"/>
@@ -2964,19 +2951,19 @@
         <v/>
       </c>
       <c r="G3" s="8" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="K3" s="8" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="L3" s="8"/>
       <c r="M3" s="8"/>
@@ -2997,7 +2984,7 @@
         <v>{"name":"param1","display":"Параметр 1"},</v>
       </c>
     </row>
-    <row r="4" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="15"/>
       <c r="B4" s="16"/>
       <c r="C4" s="16"/>
@@ -3008,19 +2995,19 @@
         <v/>
       </c>
       <c r="G4" s="8" t="s">
+        <v>254</v>
+      </c>
+      <c r="H4" s="8" t="s">
         <v>260</v>
       </c>
-      <c r="H4" s="8" t="s">
-        <v>266</v>
-      </c>
       <c r="I4" s="8" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="L4" s="8"/>
       <c r="M4" s="8"/>
@@ -3041,7 +3028,7 @@
         <v>{"name":"param2","display":"Параметр 2"},</v>
       </c>
     </row>
-    <row r="5" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="17"/>
       <c r="B5" s="18"/>
       <c r="C5" s="18"/>
@@ -3052,19 +3039,19 @@
         <v/>
       </c>
       <c r="G5" s="8" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="K5" s="8" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="L5" s="19"/>
       <c r="M5" s="19"/>
@@ -3085,9 +3072,9 @@
         <v>{"name":"param3","display":"Параметр 3"}]},</v>
       </c>
     </row>
-    <row r="6" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="12" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="B6" s="13">
         <v>2</v>
@@ -3096,10 +3083,10 @@
         <v>43</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="F6" s="13" t="str">
         <f t="shared" si="1"/>
@@ -3127,7 +3114,7 @@
         <v>{"tableid":2,"name":"Таблица ввод № 1","columns":[</v>
       </c>
     </row>
-    <row r="7" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="15"/>
       <c r="B7" s="16"/>
       <c r="C7" s="16"/>
@@ -3138,19 +3125,19 @@
         <v/>
       </c>
       <c r="G7" s="8" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="K7" s="8" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="L7" s="8"/>
       <c r="M7" s="8"/>
@@ -3171,7 +3158,7 @@
         <v>{"name":"param5","display":"Параметр 5"},</v>
       </c>
     </row>
-    <row r="8" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="15"/>
       <c r="B8" s="16"/>
       <c r="C8" s="16"/>
@@ -3182,19 +3169,19 @@
         <v/>
       </c>
       <c r="G8" s="8" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="J8" s="8" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="K8" s="8" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="L8" s="8"/>
       <c r="M8" s="8"/>
@@ -3215,7 +3202,7 @@
         <v>{"name":"param6","display":"Параметр 6"},</v>
       </c>
     </row>
-    <row r="9" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="17"/>
       <c r="B9" s="18"/>
       <c r="C9" s="18"/>
@@ -3226,19 +3213,19 @@
         <v/>
       </c>
       <c r="G9" s="8" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="J9" s="8" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="K9" s="8" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="L9" s="19"/>
       <c r="M9" s="19"/>
@@ -3259,25 +3246,25 @@
         <v>{"name":"param7","display":"Параметр 7"}]},</v>
       </c>
     </row>
-    <row r="10" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="12" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="B10" s="13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C10" s="13" t="s">
         <v>43</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="F10" s="13" t="str">
         <f t="shared" ref="F10:F13" si="2">CONCATENATE(A10,B10,C10,D10,E10)</f>
-        <v>{"tableid":2,"name":"Таблица ввод № 1","columns":[</v>
+        <v>{"tableid":3,"name":"Таблица ввод № 1","columns":[</v>
       </c>
       <c r="G10" s="8"/>
       <c r="H10" s="8"/>
@@ -3298,10 +3285,10 @@
       <c r="W10" s="14"/>
       <c r="X10" s="25" t="str">
         <f t="shared" ref="X10:X13" si="3">CONCATENATE(F10,G10,H10,I10,J10,K10,L10,M10,N10,O10,P10,Q10,R10,S10,T10,U10,V10,W10)</f>
-        <v>{"tableid":2,"name":"Таблица ввод № 1","columns":[</v>
-      </c>
-    </row>
-    <row r="11" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>{"tableid":3,"name":"Таблица ввод № 1","columns":[</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="15"/>
       <c r="B11" s="16"/>
       <c r="C11" s="16"/>
@@ -3312,19 +3299,19 @@
         <v/>
       </c>
       <c r="G11" s="8" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="J11" s="8" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="K11" s="8" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="L11" s="8"/>
       <c r="M11" s="8"/>
@@ -3345,7 +3332,7 @@
         <v>{"name":"param5","display":"Параметр 5"},</v>
       </c>
     </row>
-    <row r="12" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="15"/>
       <c r="B12" s="16"/>
       <c r="C12" s="16"/>
@@ -3356,19 +3343,19 @@
         <v/>
       </c>
       <c r="G12" s="8" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="I12" s="8" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="J12" s="8" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="K12" s="8" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="L12" s="8"/>
       <c r="M12" s="8"/>
@@ -3389,7 +3376,7 @@
         <v>{"name":"param6","display":"Параметр 6"},</v>
       </c>
     </row>
-    <row r="13" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="17"/>
       <c r="B13" s="18"/>
       <c r="C13" s="18"/>
@@ -3400,19 +3387,19 @@
         <v/>
       </c>
       <c r="G13" s="8" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="J13" s="8" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="K13" s="8" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="L13" s="19"/>
       <c r="M13" s="19"/>
@@ -3433,7 +3420,7 @@
         <v>{"name":"param7","display":"Параметр 7"},</v>
       </c>
     </row>
-    <row r="14" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="17"/>
       <c r="B14" s="18"/>
       <c r="C14" s="18"/>
@@ -3444,19 +3431,19 @@
         <v/>
       </c>
       <c r="G14" s="8" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="J14" s="8" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="K14" s="8" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="L14" s="19"/>
       <c r="M14" s="19"/>
@@ -3477,7 +3464,7 @@
         <v>{"name":"param8","display":"Параметр 8"},</v>
       </c>
     </row>
-    <row r="15" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="17"/>
       <c r="B15" s="18"/>
       <c r="C15" s="18"/>
@@ -3488,19 +3475,19 @@
         <v/>
       </c>
       <c r="G15" s="8" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="I15" s="8" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="J15" s="8" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="K15" s="8" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="L15" s="19"/>
       <c r="M15" s="19"/>
@@ -3521,7 +3508,7 @@
         <v>{"name":"param9","display":"Параметр 9"},</v>
       </c>
     </row>
-    <row r="16" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="17"/>
       <c r="B16" s="18"/>
       <c r="C16" s="18"/>
@@ -3532,19 +3519,19 @@
         <v/>
       </c>
       <c r="G16" s="8" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="J16" s="8" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="K16" s="8" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="L16" s="19"/>
       <c r="M16" s="19"/>
@@ -3565,7 +3552,7 @@
         <v>{"name":"param10","display":"Параметр 10"},</v>
       </c>
     </row>
-    <row r="17" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="17"/>
       <c r="B17" s="18"/>
       <c r="C17" s="18"/>
@@ -3576,19 +3563,19 @@
         <v/>
       </c>
       <c r="G17" s="8" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="H17" s="8" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="J17" s="8" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="K17" s="8" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="L17" s="19"/>
       <c r="M17" s="19"/>
@@ -3609,7 +3596,7 @@
         <v>{"name":"param11","display":"Параметр 11"},</v>
       </c>
     </row>
-    <row r="18" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="17"/>
       <c r="B18" s="18"/>
       <c r="C18" s="18"/>
@@ -3620,19 +3607,19 @@
         <v/>
       </c>
       <c r="G18" s="8" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="H18" s="8" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="J18" s="8" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="K18" s="8" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="L18" s="19"/>
       <c r="M18" s="19"/>
@@ -3653,7 +3640,7 @@
         <v>{"name":"param12","display":"Параметр 12"},</v>
       </c>
     </row>
-    <row r="19" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="17"/>
       <c r="B19" s="18"/>
       <c r="C19" s="18"/>
@@ -3664,19 +3651,19 @@
         <v/>
       </c>
       <c r="G19" s="8" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="H19" s="8" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="J19" s="8" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="K19" s="8" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="L19" s="19"/>
       <c r="M19" s="19"/>
@@ -3697,7 +3684,7 @@
         <v>{"name":"param13","display":"Параметр 13"},</v>
       </c>
     </row>
-    <row r="20" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="17"/>
       <c r="B20" s="18"/>
       <c r="C20" s="18"/>
@@ -3708,19 +3695,19 @@
         <v/>
       </c>
       <c r="G20" s="8" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="J20" s="8" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="K20" s="8" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="L20" s="19"/>
       <c r="M20" s="19"/>
@@ -3741,7 +3728,7 @@
         <v>{"name":"param14","display":"Параметр 14"},</v>
       </c>
     </row>
-    <row r="21" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="17"/>
       <c r="B21" s="18"/>
       <c r="C21" s="18"/>
@@ -3752,19 +3739,19 @@
         <v/>
       </c>
       <c r="G21" s="8" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="H21" s="8" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="I21" s="8" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="J21" s="8" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="K21" s="8" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="L21" s="19"/>
       <c r="M21" s="19"/>
@@ -3798,26 +3785,26 @@
       <selection activeCell="P26" sqref="P26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="90.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="132.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="90.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="132.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:16" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="28" t="s">
         <v>21</v>
       </c>
@@ -3863,7 +3850,7 @@
         <v>["flid":flid"koef":koef"leadPt":leadPt"leadStat":leadStat</v>
       </c>
     </row>
-    <row r="3" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="1">
         <v>1</v>
       </c>
@@ -3896,7 +3883,7 @@
         <v>{ "flid" :1, "eic":"XXX-YYY-000-ZZZ-001", "name":"Харьков ГРС 1 ", "chid": 1, "cfgLines": null},</v>
       </c>
     </row>
-    <row r="4" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="1">
         <v>2</v>
       </c>
@@ -3929,7 +3916,7 @@
         <v>{ "flid" :2, "eic":"XXX-YYY-000-ZZZ-002", "name":"Харьков ГРС 2", "chid": 2, "cfgLines": null},</v>
       </c>
     </row>
-    <row r="5" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="1">
         <v>3</v>
       </c>
@@ -3962,7 +3949,7 @@
         <v>{ "flid" :3, "eic":"XXX-YYY-000-ZZZ-003", "name":"Харьков ГРС 3", "chid": 3, "cfgLines": null},</v>
       </c>
     </row>
-    <row r="6" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="1">
         <v>4</v>
       </c>
@@ -3995,7 +3982,7 @@
         <v>{ "flid" :4, "eic":"XXX-YYY-000-ZZZ-004", "name":"Харьков ГРС 4", "chid": 4, "cfgLines": null},</v>
       </c>
     </row>
-    <row r="7" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="1">
         <v>5</v>
       </c>
@@ -4028,7 +4015,7 @@
         <v>{ "flid" :5, "eic":"XXX-YYY-000-ZZZ-005", "name":"Харьков ГРС 5", "chid": 5, "cfgLines": null},</v>
       </c>
     </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B8" s="1">
         <v>6</v>
       </c>
@@ -4061,7 +4048,7 @@
         <v>{ "flid" :6, "eic":"XXX-YYY-000-ZZZ-006", "name":"Харьков ГРС 6", "chid": 6, "cfgLines": null},</v>
       </c>
     </row>
-    <row r="9" spans="2:16" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -4077,7 +4064,7 @@
       <c r="O9" s="10"/>
       <c r="P9" s="34"/>
     </row>
-    <row r="10" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="1">
         <v>7</v>
       </c>
@@ -4110,7 +4097,7 @@
         <v>{ "flid" :7, "eic":"XXX-YYY-000-ZZZ-007", "name":"Харьков ГРС 7", "chid": null, "cfgLines": [</v>
       </c>
     </row>
-    <row r="11" spans="2:16" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -4148,7 +4135,7 @@
         <v>{"flid":1,"koef":1,"leadPt":false,"leadStat":false},</v>
       </c>
     </row>
-    <row r="12" spans="2:16" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -4186,7 +4173,7 @@
         <v>{"flid":2,"koef":1,"leadPt":false,"leadStat":false},</v>
       </c>
     </row>
-    <row r="13" spans="2:16" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -4224,7 +4211,7 @@
         <v>{"flid":3,"koef":1,"leadPt":false,"leadStat":false},</v>
       </c>
     </row>
-    <row r="14" spans="2:16" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -4262,7 +4249,7 @@
         <v>{"flid":4,"koef":1,"leadPt":false,"leadStat":false}]},</v>
       </c>
     </row>
-    <row r="15" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="1">
         <v>8</v>
       </c>
@@ -4295,7 +4282,7 @@
         <v>{ "flid" :8, "eic":"XXX-YYY-000-ZZZ-008", "name":"Харьков ГРС 8", "chid": null, "cfgLines": [</v>
       </c>
     </row>
-    <row r="16" spans="2:16" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -4333,7 +4320,7 @@
         <v>{"flid":1,"koef":1,"leadPt":false,"leadStat":false},</v>
       </c>
     </row>
-    <row r="17" spans="2:16" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -4371,7 +4358,7 @@
         <v>{"flid":2,"koef":1,"leadPt":false,"leadStat":false},</v>
       </c>
     </row>
-    <row r="18" spans="2:16" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -4409,7 +4396,7 @@
         <v>{"flid":3,"koef":1,"leadPt":false,"leadStat":false},</v>
       </c>
     </row>
-    <row r="19" spans="2:16" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -4461,20 +4448,20 @@
       <selection sqref="A1:XFD6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.5703125" customWidth="1"/>
+    <col min="1" max="1" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.5546875" customWidth="1"/>
     <col min="8" max="8" width="22" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="105.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="105.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15" x14ac:dyDescent="0.3">
       <c r="H1" s="29" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="15" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>21</v>
       </c>
@@ -4506,7 +4493,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="15" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -4539,7 +4526,7 @@
         <v>{ "flid": 1,"chid":1, "p": 50, "t" :30,"dp": 1000, "q":100, "currday":1000, "lastupdate":"2020-02-19T12:01", "quality":192},</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="15" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -4572,7 +4559,7 @@
         <v>{ "flid": 1,"chid":1, "p": 50, "t" :30,"dp": 1000, "q":100, "currday":1000, "lastupdate":"2020-02-19T13:02", "quality":192},</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="15" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -4605,7 +4592,7 @@
         <v>{ "flid": 1,"chid":1, "p": 50, "t" :30,"dp": 1000, "q":100, "currday":1000, "lastupdate":"2020-02-19T12:02", "quality":192},</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="15" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>1</v>
       </c>
@@ -4638,7 +4625,7 @@
         <v>{ "flid": 1,"chid":1, "p": 50, "t" :30,"dp": 1000, "q":100, "currday":1000, "lastupdate":"2020-02-19T13:03", "quality":192},</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="15" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>1</v>
       </c>
@@ -4671,7 +4658,7 @@
         <v>{ "flid": 1,"chid":1, "p": 50, "t" :30,"dp": 1000, "q":100, "currday":1000, "lastupdate":"2020-02-19T12:03", "quality":192},</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="15" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>1</v>
       </c>
@@ -4704,7 +4691,7 @@
         <v>{ "flid": 1,"chid":1, "p": 50, "t" :30,"dp": 1000, "q":100, "currday":1000, "lastupdate":"2020-02-19T13:04", "quality":192},</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="15" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>1</v>
       </c>
@@ -4737,7 +4724,7 @@
         <v>{ "flid": 1,"chid":1, "p": 50, "t" :30,"dp": 1000, "q":100, "currday":1000, "lastupdate":"2020-02-19T12:04", "quality":192},</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="15" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>1</v>
       </c>
@@ -4770,7 +4757,7 @@
         <v>{ "flid": 1,"chid":1, "p": 50, "t" :30,"dp": 1000, "q":100, "currday":1000, "lastupdate":"2020-02-19T13:05", "quality":192},</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="15" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>1</v>
       </c>
@@ -4803,7 +4790,7 @@
         <v>{ "flid": 1,"chid":1, "p": 50, "t" :30,"dp": 1000, "q":100, "currday":1000, "lastupdate":"2020-02-19T12:05", "quality":192},</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="15" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>2</v>
       </c>
@@ -4836,7 +4823,7 @@
         <v>{ "flid": 2,"chid":2, "p": 50, "t" :30,"dp": 1000, "q":100, "currday":1000, "lastupdate":"2020-02-19T12:01", "quality":192},</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="15" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>2</v>
       </c>
@@ -4869,7 +4856,7 @@
         <v>{ "flid": 2,"chid":2, "p": 50, "t" :30,"dp": 1000, "q":100, "currday":1000, "lastupdate":"2020-02-19T13:02", "quality":192},</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" ht="15" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>2</v>
       </c>
@@ -4902,7 +4889,7 @@
         <v>{ "flid": 2,"chid":2, "p": 50, "t" :30,"dp": 1000, "q":100, "currday":1000, "lastupdate":"2020-02-19T12:02", "quality":192},</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" ht="15" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>2</v>
       </c>
@@ -4935,7 +4922,7 @@
         <v>{ "flid": 2,"chid":2, "p": 50, "t" :30,"dp": 1000, "q":100, "currday":1000, "lastupdate":"2020-02-19T13:03", "quality":192},</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" ht="15" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>2</v>
       </c>
@@ -4968,7 +4955,7 @@
         <v>{ "flid": 2,"chid":2, "p": 50, "t" :30,"dp": 1000, "q":100, "currday":1000, "lastupdate":"2020-02-19T12:03", "quality":192},</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" ht="15" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>2</v>
       </c>
@@ -5001,7 +4988,7 @@
         <v>{ "flid": 2,"chid":2, "p": 50, "t" :30,"dp": 1000, "q":100, "currday":1000, "lastupdate":"2020-02-19T13:04", "quality":192},</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" ht="15" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>2</v>
       </c>
@@ -5034,7 +5021,7 @@
         <v>{ "flid": 2,"chid":2, "p": 50, "t" :30,"dp": 1000, "q":100, "currday":1000, "lastupdate":"2020-02-19T12:04", "quality":192},</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" ht="15" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>2</v>
       </c>
@@ -5067,7 +5054,7 @@
         <v>{ "flid": 2,"chid":2, "p": 50, "t" :30,"dp": 1000, "q":100, "currday":1000, "lastupdate":"2020-02-19T13:05", "quality":192},</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" ht="15" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>2</v>
       </c>
@@ -5100,7 +5087,7 @@
         <v>{ "flid": 2,"chid":2, "p": 50, "t" :30,"dp": 1000, "q":100, "currday":1000, "lastupdate":"2020-02-19T12:05", "quality":192},</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" ht="15" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>3</v>
       </c>
@@ -5133,7 +5120,7 @@
         <v>{ "flid": 3,"chid":3, "p": 50, "t" :30,"dp": 1000, "q":100, "currday":1000, "lastupdate":"2020-02-19T12:01", "quality":192},</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" ht="15" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>3</v>
       </c>
@@ -5166,7 +5153,7 @@
         <v>{ "flid": 3,"chid":3, "p": 50, "t" :30,"dp": 1000, "q":100, "currday":1000, "lastupdate":"2020-02-19T13:02", "quality":192},</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>3</v>
       </c>
@@ -5199,7 +5186,7 @@
         <v>{ "flid": 3,"chid":3, "p": 50, "t" :30,"dp": 1000, "q":100, "currday":1000, "lastupdate":"2020-02-19T12:02", "quality":192},</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>3</v>
       </c>
@@ -5232,7 +5219,7 @@
         <v>{ "flid": 3,"chid":3, "p": 50, "t" :30,"dp": 1000, "q":100, "currday":1000, "lastupdate":"2020-02-19T13:03", "quality":192},</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>3</v>
       </c>
@@ -5265,7 +5252,7 @@
         <v>{ "flid": 3,"chid":3, "p": 50, "t" :30,"dp": 1000, "q":100, "currday":1000, "lastupdate":"2020-02-19T12:03", "quality":192},</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>3</v>
       </c>
@@ -5298,7 +5285,7 @@
         <v>{ "flid": 3,"chid":3, "p": 50, "t" :30,"dp": 1000, "q":100, "currday":1000, "lastupdate":"2020-02-19T13:04", "quality":192},</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>3</v>
       </c>
@@ -5331,7 +5318,7 @@
         <v>{ "flid": 3,"chid":3, "p": 50, "t" :30,"dp": 1000, "q":100, "currday":1000, "lastupdate":"2020-02-19T12:04", "quality":192},</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>3</v>
       </c>
@@ -5364,7 +5351,7 @@
         <v>{ "flid": 3,"chid":3, "p": 50, "t" :30,"dp": 1000, "q":100, "currday":1000, "lastupdate":"2020-02-19T13:05", "quality":192},</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>3</v>
       </c>
@@ -5397,7 +5384,7 @@
         <v>{ "flid": 3,"chid":3, "p": 50, "t" :30,"dp": 1000, "q":100, "currday":1000, "lastupdate":"2020-02-19T12:05", "quality":192},</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>4</v>
       </c>
@@ -5430,7 +5417,7 @@
         <v>{ "flid": 4,"chid":4, "p": 50, "t" :30,"dp": 1000, "q":100, "currday":1000, "lastupdate":"2020-02-19T12:01", "quality":192},</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>4</v>
       </c>
@@ -5463,7 +5450,7 @@
         <v>{ "flid": 4,"chid":4, "p": 50, "t" :30,"dp": 1000, "q":100, "currday":1000, "lastupdate":"2020-02-19T13:02", "quality":192},</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>4</v>
       </c>
@@ -5496,7 +5483,7 @@
         <v>{ "flid": 4,"chid":4, "p": 50, "t" :30,"dp": 1000, "q":100, "currday":1000, "lastupdate":"2020-02-19T12:02", "quality":192},</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>4</v>
       </c>
@@ -5529,7 +5516,7 @@
         <v>{ "flid": 4,"chid":4, "p": 50, "t" :30,"dp": 1000, "q":100, "currday":1000, "lastupdate":"2020-02-19T13:03", "quality":192},</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>4</v>
       </c>
@@ -5562,7 +5549,7 @@
         <v>{ "flid": 4,"chid":4, "p": 50, "t" :30,"dp": 1000, "q":100, "currday":1000, "lastupdate":"2020-02-19T12:03", "quality":192},</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>4</v>
       </c>
@@ -5595,7 +5582,7 @@
         <v>{ "flid": 4,"chid":4, "p": 50, "t" :30,"dp": 1000, "q":100, "currday":1000, "lastupdate":"2020-02-19T13:04", "quality":192},</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>4</v>
       </c>
@@ -5628,7 +5615,7 @@
         <v>{ "flid": 4,"chid":4, "p": 50, "t" :30,"dp": 1000, "q":100, "currday":1000, "lastupdate":"2020-02-19T12:04", "quality":192},</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>4</v>
       </c>
@@ -5661,7 +5648,7 @@
         <v>{ "flid": 4,"chid":4, "p": 50, "t" :30,"dp": 1000, "q":100, "currday":1000, "lastupdate":"2020-02-19T13:05", "quality":192},</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>4</v>
       </c>
@@ -5694,7 +5681,7 @@
         <v>{ "flid": 4,"chid":4, "p": 50, "t" :30,"dp": 1000, "q":100, "currday":1000, "lastupdate":"2020-02-19T12:05", "quality":192},</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -5705,7 +5692,7 @@
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -5730,24 +5717,24 @@
       <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="4" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="4" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="8.5546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="22" customWidth="1"/>
-    <col min="10" max="10" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="145.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="145.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="H1" s="29" t="s">
         <v>20</v>
       </c>
       <c r="I1" s="29"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>21</v>
       </c>
@@ -5780,7 +5767,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="47" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" s="47" customFormat="1" ht="15" x14ac:dyDescent="0.3">
       <c r="A3" s="46">
         <v>1</v>
       </c>
@@ -5814,7 +5801,7 @@
         <v>{ "flid": 1,"chid":1, "p": 50, "t" :30,"dp": 1000, "q":100, "start":"2020-02-19T12:00", "lastupdate":"2020-02-19T13:00", "quality":192},</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="47" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" s="47" customFormat="1" ht="15" x14ac:dyDescent="0.3">
       <c r="A4" s="46">
         <v>1</v>
       </c>
@@ -5848,7 +5835,7 @@
         <v>{ "flid": 1,"chid":1, "p": 50, "t" :30,"dp": 1000, "q":100, "start":"2020-02-19T13:00", "lastupdate":"2020-02-19T14:00", "quality":192},</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="47" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" s="47" customFormat="1" ht="15" x14ac:dyDescent="0.3">
       <c r="A5" s="46">
         <v>1</v>
       </c>
@@ -5882,7 +5869,7 @@
         <v>{ "flid": 1,"chid":1, "p": 50, "t" :30,"dp": 1000, "q":100, "start":"2020-02-19T14:00", "lastupdate":"2020-02-19T15:00", "quality":192},</v>
       </c>
     </row>
-    <row r="6" spans="1:11" s="47" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" s="47" customFormat="1" ht="15" x14ac:dyDescent="0.3">
       <c r="A6" s="46">
         <v>1</v>
       </c>
@@ -5916,7 +5903,7 @@
         <v>{ "flid": 1,"chid":1, "p": 50, "t" :30,"dp": 1000, "q":100, "start":"2020-02-19T15:00", "lastupdate":"2020-02-19T16:00", "quality":192},</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="47" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" s="47" customFormat="1" ht="15" x14ac:dyDescent="0.3">
       <c r="A7" s="46">
         <v>1</v>
       </c>
@@ -5950,7 +5937,7 @@
         <v>{ "flid": 1,"chid":1, "p": 50, "t" :30,"dp": 1000, "q":100, "start":"2020-02-19T16:00", "lastupdate":"2020-02-19T17:00", "quality":192},</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="47" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" s="47" customFormat="1" ht="15" x14ac:dyDescent="0.3">
       <c r="A8" s="46">
         <v>1</v>
       </c>
@@ -5984,7 +5971,7 @@
         <v>{ "flid": 1,"chid":1, "p": 50, "t" :30,"dp": 1000, "q":100, "start":"2020-02-19T17:00", "lastupdate":"2020-02-19T18:00", "quality":192},</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="47" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" s="47" customFormat="1" ht="15" x14ac:dyDescent="0.3">
       <c r="A9" s="46">
         <v>1</v>
       </c>
@@ -6018,7 +6005,7 @@
         <v>{ "flid": 1,"chid":1, "p": 50, "t" :30,"dp": 1000, "q":100, "start":"2020-02-19T18:00", "lastupdate":"2020-02-19T19:00", "quality":192},</v>
       </c>
     </row>
-    <row r="10" spans="1:11" s="47" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" s="47" customFormat="1" ht="15" x14ac:dyDescent="0.3">
       <c r="A10" s="46">
         <v>1</v>
       </c>
@@ -6052,7 +6039,7 @@
         <v>{ "flid": 1,"chid":1, "p": 50, "t" :30,"dp": 1000, "q":100, "start":"2020-02-19T19:00", "lastupdate":"2020-02-19T20:00", "quality":192},</v>
       </c>
     </row>
-    <row r="11" spans="1:11" s="47" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" s="47" customFormat="1" ht="15" x14ac:dyDescent="0.3">
       <c r="A11" s="46">
         <v>1</v>
       </c>
@@ -6086,7 +6073,7 @@
         <v>{ "flid": 1,"chid":1, "p": 50, "t" :30,"dp": 1000, "q":100, "start":"2020-02-19T20:00", "lastupdate":"2020-02-19T21:00", "quality":192},</v>
       </c>
     </row>
-    <row r="12" spans="1:11" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" s="49" customFormat="1" ht="15" x14ac:dyDescent="0.3">
       <c r="A12" s="48">
         <v>2</v>
       </c>
@@ -6120,7 +6107,7 @@
         <v>{ "flid": 2,"chid":2, "p": 50, "t" :30,"dp": 1000, "q":100, "start":"2020-02-19T12:00", "lastupdate":"2020-02-19T13:00", "quality":192},</v>
       </c>
     </row>
-    <row r="13" spans="1:11" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" s="49" customFormat="1" ht="15" x14ac:dyDescent="0.3">
       <c r="A13" s="48">
         <v>2</v>
       </c>
@@ -6154,7 +6141,7 @@
         <v>{ "flid": 2,"chid":2, "p": 50, "t" :30,"dp": 1000, "q":100, "start":"2020-02-19T13:00", "lastupdate":"2020-02-19T14:00", "quality":192},</v>
       </c>
     </row>
-    <row r="14" spans="1:11" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" s="49" customFormat="1" ht="15" x14ac:dyDescent="0.3">
       <c r="A14" s="48">
         <v>2</v>
       </c>
@@ -6188,7 +6175,7 @@
         <v>{ "flid": 2,"chid":2, "p": 50, "t" :30,"dp": 1000, "q":100, "start":"2020-02-19T14:00", "lastupdate":"2020-02-19T15:00", "quality":192},</v>
       </c>
     </row>
-    <row r="15" spans="1:11" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" s="49" customFormat="1" ht="15" x14ac:dyDescent="0.3">
       <c r="A15" s="48">
         <v>2</v>
       </c>
@@ -6222,7 +6209,7 @@
         <v>{ "flid": 2,"chid":2, "p": 50, "t" :30,"dp": 1000, "q":100, "start":"2020-02-19T15:00", "lastupdate":"2020-02-19T16:00", "quality":192},</v>
       </c>
     </row>
-    <row r="16" spans="1:11" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" s="49" customFormat="1" ht="15" x14ac:dyDescent="0.3">
       <c r="A16" s="48">
         <v>2</v>
       </c>
@@ -6256,7 +6243,7 @@
         <v>{ "flid": 2,"chid":2, "p": 50, "t" :30,"dp": 1000, "q":100, "start":"2020-02-19T16:00", "lastupdate":"2020-02-19T17:00", "quality":192},</v>
       </c>
     </row>
-    <row r="17" spans="1:11" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" s="49" customFormat="1" ht="15" x14ac:dyDescent="0.3">
       <c r="A17" s="48">
         <v>2</v>
       </c>
@@ -6290,7 +6277,7 @@
         <v>{ "flid": 2,"chid":2, "p": 50, "t" :30,"dp": 1000, "q":100, "start":"2020-02-19T17:00", "lastupdate":"2020-02-19T18:00", "quality":192},</v>
       </c>
     </row>
-    <row r="18" spans="1:11" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" s="49" customFormat="1" ht="15" x14ac:dyDescent="0.3">
       <c r="A18" s="48">
         <v>2</v>
       </c>
@@ -6324,7 +6311,7 @@
         <v>{ "flid": 2,"chid":2, "p": 50, "t" :30,"dp": 1000, "q":100, "start":"2020-02-19T18:00", "lastupdate":"2020-02-19T19:00", "quality":192},</v>
       </c>
     </row>
-    <row r="19" spans="1:11" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" s="49" customFormat="1" ht="15" x14ac:dyDescent="0.3">
       <c r="A19" s="48">
         <v>2</v>
       </c>
@@ -6358,7 +6345,7 @@
         <v>{ "flid": 2,"chid":2, "p": 50, "t" :30,"dp": 1000, "q":100, "start":"2020-02-19T19:00", "lastupdate":"2020-02-19T20:00", "quality":192},</v>
       </c>
     </row>
-    <row r="20" spans="1:11" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" s="49" customFormat="1" ht="15" x14ac:dyDescent="0.3">
       <c r="A20" s="48">
         <v>2</v>
       </c>
@@ -6392,7 +6379,7 @@
         <v>{ "flid": 2,"chid":2, "p": 50, "t" :30,"dp": 1000, "q":100, "start":"2020-02-19T20:00", "lastupdate":"2020-02-19T21:00", "quality":192},</v>
       </c>
     </row>
-    <row r="21" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" s="51" customFormat="1" ht="15" x14ac:dyDescent="0.3">
       <c r="A21" s="50">
         <v>3</v>
       </c>
@@ -6426,7 +6413,7 @@
         <v>{ "flid": 3,"chid":3, "p": 50, "t" :30,"dp": 1000, "q":100, "start":"2020-02-19T12:00", "lastupdate":"2020-02-19T13:00", "quality":192},</v>
       </c>
     </row>
-    <row r="22" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="50">
         <v>3</v>
       </c>
@@ -6460,7 +6447,7 @@
         <v>{ "flid": 3,"chid":3, "p": 50, "t" :30,"dp": 1000, "q":100, "start":"2020-02-19T13:00", "lastupdate":"2020-02-19T14:00", "quality":193},</v>
       </c>
     </row>
-    <row r="23" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="50">
         <v>3</v>
       </c>
@@ -6494,7 +6481,7 @@
         <v>{ "flid": 3,"chid":3, "p": 50, "t" :30,"dp": 1000, "q":100, "start":"2020-02-19T14:00", "lastupdate":"2020-02-19T15:00", "quality":194},</v>
       </c>
     </row>
-    <row r="24" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="50">
         <v>3</v>
       </c>
@@ -6528,7 +6515,7 @@
         <v>{ "flid": 3,"chid":3, "p": 50, "t" :30,"dp": 1000, "q":100, "start":"2020-02-19T15:00", "lastupdate":"2020-02-19T16:00", "quality":195},</v>
       </c>
     </row>
-    <row r="25" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="50">
         <v>3</v>
       </c>
@@ -6562,7 +6549,7 @@
         <v>{ "flid": 3,"chid":3, "p": 50, "t" :30,"dp": 1000, "q":100, "start":"2020-02-19T16:00", "lastupdate":"2020-02-19T17:00", "quality":196},</v>
       </c>
     </row>
-    <row r="26" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="50">
         <v>3</v>
       </c>
@@ -6596,7 +6583,7 @@
         <v>{ "flid": 3,"chid":3, "p": 50, "t" :30,"dp": 1000, "q":100, "start":"2020-02-19T17:00", "lastupdate":"2020-02-19T18:00", "quality":197},</v>
       </c>
     </row>
-    <row r="27" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="50">
         <v>3</v>
       </c>
@@ -6630,7 +6617,7 @@
         <v>{ "flid": 3,"chid":3, "p": 50, "t" :30,"dp": 1000, "q":100, "start":"2020-02-19T18:00", "lastupdate":"2020-02-19T19:00", "quality":198},</v>
       </c>
     </row>
-    <row r="28" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="50">
         <v>3</v>
       </c>
@@ -6664,7 +6651,7 @@
         <v>{ "flid": 3,"chid":3, "p": 50, "t" :30,"dp": 1000, "q":100, "start":"2020-02-19T19:00", "lastupdate":"2020-02-19T20:00", "quality":199},</v>
       </c>
     </row>
-    <row r="29" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="50">
         <v>3</v>
       </c>
@@ -6698,7 +6685,7 @@
         <v>{ "flid": 3,"chid":3, "p": 50, "t" :30,"dp": 1000, "q":100, "start":"2020-02-19T20:00", "lastupdate":"2020-02-19T21:00", "quality":200},</v>
       </c>
     </row>
-    <row r="30" spans="1:11" s="49" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="48">
         <v>4</v>
       </c>
@@ -6732,7 +6719,7 @@
         <v>{ "flid": 4,"chid":4, "p": 50, "t" :30,"dp": 1000, "q":100, "start":"2020-02-19T12:00", "lastupdate":"2020-02-19T13:00", "quality":201},</v>
       </c>
     </row>
-    <row r="31" spans="1:11" s="49" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="48">
         <v>4</v>
       </c>
@@ -6766,7 +6753,7 @@
         <v>{ "flid": 4,"chid":4, "p": 50, "t" :30,"dp": 1000, "q":100, "start":"2020-02-19T13:00", "lastupdate":"2020-02-19T14:00", "quality":202},</v>
       </c>
     </row>
-    <row r="32" spans="1:11" s="49" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="48">
         <v>4</v>
       </c>
@@ -6800,7 +6787,7 @@
         <v>{ "flid": 4,"chid":4, "p": 50, "t" :30,"dp": 1000, "q":100, "start":"2020-02-19T14:00", "lastupdate":"2020-02-19T15:00", "quality":203},</v>
       </c>
     </row>
-    <row r="33" spans="1:11" s="49" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="48">
         <v>4</v>
       </c>
@@ -6834,7 +6821,7 @@
         <v>{ "flid": 4,"chid":4, "p": 50, "t" :30,"dp": 1000, "q":100, "start":"2020-02-19T15:00", "lastupdate":"2020-02-19T16:00", "quality":204},</v>
       </c>
     </row>
-    <row r="34" spans="1:11" s="49" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="48">
         <v>4</v>
       </c>
@@ -6868,7 +6855,7 @@
         <v>{ "flid": 4,"chid":4, "p": 50, "t" :30,"dp": 1000, "q":100, "start":"2020-02-19T16:00", "lastupdate":"2020-02-19T17:00", "quality":205},</v>
       </c>
     </row>
-    <row r="35" spans="1:11" s="49" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="48">
         <v>4</v>
       </c>
@@ -6902,7 +6889,7 @@
         <v>{ "flid": 4,"chid":4, "p": 50, "t" :30,"dp": 1000, "q":100, "start":"2020-02-19T17:00", "lastupdate":"2020-02-19T18:00", "quality":206},</v>
       </c>
     </row>
-    <row r="36" spans="1:11" s="49" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="48">
         <v>4</v>
       </c>
@@ -6936,7 +6923,7 @@
         <v>{ "flid": 4,"chid":4, "p": 50, "t" :30,"dp": 1000, "q":100, "start":"2020-02-19T18:00", "lastupdate":"2020-02-19T19:00", "quality":207},</v>
       </c>
     </row>
-    <row r="37" spans="1:11" s="49" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="48">
         <v>4</v>
       </c>
@@ -6970,7 +6957,7 @@
         <v>{ "flid": 4,"chid":4, "p": 50, "t" :30,"dp": 1000, "q":100, "start":"2020-02-19T19:00", "lastupdate":"2020-02-19T20:00", "quality":208},</v>
       </c>
     </row>
-    <row r="38" spans="1:11" s="49" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="48">
         <v>4</v>
       </c>
@@ -7004,7 +6991,7 @@
         <v>{ "flid": 4,"chid":4, "p": 50, "t" :30,"dp": 1000, "q":100, "start":"2020-02-19T20:00", "lastupdate":"2020-02-19T21:00", "quality":209},</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="J39" s="1"/>
     </row>
   </sheetData>
@@ -7020,20 +7007,20 @@
       <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.5546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="H1" s="29" t="s">
         <v>20</v>
       </c>
       <c r="I1" s="29"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>21</v>
       </c>
@@ -7066,7 +7053,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -7100,7 +7087,7 @@
         <v>{ "flid": 1,"chid":1, "p": 50, "t" :30,"dp": 1000, "q":100, "start":"2020-02-01T07:00", "lastupdate":"2020-02-02T07:00", "quality":192},</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -7134,7 +7121,7 @@
         <v>{ "flid": 1,"chid":1, "p": 50, "t" :30,"dp": 1000, "q":100, "start":"2020-02-02T07:00", "lastupdate":"2020-02-03T07:00", "quality":192},</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -7168,7 +7155,7 @@
         <v>{ "flid": 1,"chid":1, "p": 50, "t" :30,"dp": 1000, "q":100, "start":"2020-02-03T07:00", "lastupdate":"2020-02-04T07:00", "quality":192},</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>1</v>
       </c>
@@ -7202,7 +7189,7 @@
         <v>{ "flid": 1,"chid":1, "p": 50, "t" :30,"dp": 1000, "q":100, "start":"2020-02-04T07:00", "lastupdate":"2020-02-05T07:00", "quality":192},</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>1</v>
       </c>
@@ -7236,7 +7223,7 @@
         <v>{ "flid": 1,"chid":1, "p": 50, "t" :30,"dp": 1000, "q":100, "start":"2020-02-05T07:00", "lastupdate":"2020-02-06T07:00", "quality":192},</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>1</v>
       </c>
@@ -7270,7 +7257,7 @@
         <v>{ "flid": 1,"chid":1, "p": 50, "t" :30,"dp": 1000, "q":100, "start":"2020-02-06T07:00", "lastupdate":"2020-02-07T07:00", "quality":192},</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>1</v>
       </c>
@@ -7304,7 +7291,7 @@
         <v>{ "flid": 1,"chid":1, "p": 50, "t" :30,"dp": 1000, "q":100, "start":"2020-02-07T07:00", "lastupdate":"2020-02-08T07:00", "quality":192},</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>1</v>
       </c>
@@ -7338,7 +7325,7 @@
         <v>{ "flid": 1,"chid":1, "p": 50, "t" :30,"dp": 1000, "q":100, "start":"2020-02-08T07:00", "lastupdate":"2020-02-09T07:00", "quality":192},</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>1</v>
       </c>
@@ -7372,7 +7359,7 @@
         <v>{ "flid": 1,"chid":1, "p": 50, "t" :30,"dp": 1000, "q":100, "start":"2020-02-09T07:00", "lastupdate":"2020-02-10T07:00", "quality":192},</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>2</v>
       </c>
@@ -7406,7 +7393,7 @@
         <v>{ "flid": 2,"chid":2, "p": 50, "t" :30,"dp": 1000, "q":100, "start":"2020-02-01T07:00", "lastupdate":"2020-02-02T07:00", "quality":192},</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>2</v>
       </c>
@@ -7440,7 +7427,7 @@
         <v>{ "flid": 2,"chid":2, "p": 50, "t" :30,"dp": 1000, "q":100, "start":"2020-02-02T07:00", "lastupdate":"2020-02-03T07:00", "quality":192},</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>2</v>
       </c>
@@ -7474,7 +7461,7 @@
         <v>{ "flid": 2,"chid":2, "p": 50, "t" :30,"dp": 1000, "q":100, "start":"2020-02-03T07:00", "lastupdate":"2020-02-04T07:00", "quality":192},</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>2</v>
       </c>
@@ -7508,7 +7495,7 @@
         <v>{ "flid": 2,"chid":2, "p": 50, "t" :30,"dp": 1000, "q":100, "start":"2020-02-04T07:00", "lastupdate":"2020-02-05T07:00", "quality":192},</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>2</v>
       </c>
@@ -7542,7 +7529,7 @@
         <v>{ "flid": 2,"chid":2, "p": 50, "t" :30,"dp": 1000, "q":100, "start":"2020-02-05T07:00", "lastupdate":"2020-02-06T07:00", "quality":192},</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>2</v>
       </c>
@@ -7576,7 +7563,7 @@
         <v>{ "flid": 2,"chid":2, "p": 50, "t" :30,"dp": 1000, "q":100, "start":"2020-02-06T07:00", "lastupdate":"2020-02-07T07:00", "quality":192},</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>2</v>
       </c>
@@ -7610,7 +7597,7 @@
         <v>{ "flid": 2,"chid":2, "p": 50, "t" :30,"dp": 1000, "q":100, "start":"2020-02-07T07:00", "lastupdate":"2020-02-08T07:00", "quality":192},</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>2</v>
       </c>
@@ -7644,7 +7631,7 @@
         <v>{ "flid": 2,"chid":2, "p": 50, "t" :30,"dp": 1000, "q":100, "start":"2020-02-08T07:00", "lastupdate":"2020-02-09T07:00", "quality":192},</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>2</v>
       </c>
@@ -7678,7 +7665,7 @@
         <v>{ "flid": 2,"chid":2, "p": 50, "t" :30,"dp": 1000, "q":100, "start":"2020-02-09T07:00", "lastupdate":"2020-02-10T07:00", "quality":192},</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" ht="15" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>3</v>
       </c>
@@ -7712,7 +7699,7 @@
         <v>{ "flid": 3,"chid":3, "p": 50, "t" :30,"dp": 1000, "q":100, "start":"2020-02-01T07:00", "lastupdate":"2020-02-02T07:00", "quality":192},</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>3</v>
       </c>
@@ -7745,7 +7732,7 @@
         <v>{ "flid": 3,"chid":3, "p": 50, "t" :30,"dp": 1000, "q":100, "start":"2020-02-02T07:00", "lastupdate":"2020-02-03T07:00", "quality":192},</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>3</v>
       </c>
@@ -7778,7 +7765,7 @@
         <v>{ "flid": 3,"chid":3, "p": 50, "t" :30,"dp": 1000, "q":100, "start":"2020-02-03T07:00", "lastupdate":"2020-02-04T07:00", "quality":192},</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>3</v>
       </c>
@@ -7811,7 +7798,7 @@
         <v>{ "flid": 3,"chid":3, "p": 50, "t" :30,"dp": 1000, "q":100, "start":"2020-02-04T07:00", "lastupdate":"2020-02-05T07:00", "quality":192},</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>3</v>
       </c>
@@ -7844,7 +7831,7 @@
         <v>{ "flid": 3,"chid":3, "p": 50, "t" :30,"dp": 1000, "q":100, "start":"2020-02-05T07:00", "lastupdate":"2020-02-06T07:00", "quality":192},</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>3</v>
       </c>
@@ -7877,7 +7864,7 @@
         <v>{ "flid": 3,"chid":3, "p": 50, "t" :30,"dp": 1000, "q":100, "start":"2020-02-06T07:00", "lastupdate":"2020-02-07T07:00", "quality":192},</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>3</v>
       </c>
@@ -7910,7 +7897,7 @@
         <v>{ "flid": 3,"chid":3, "p": 50, "t" :30,"dp": 1000, "q":100, "start":"2020-02-07T07:00", "lastupdate":"2020-02-08T07:00", "quality":192},</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>3</v>
       </c>
@@ -7943,7 +7930,7 @@
         <v>{ "flid": 3,"chid":3, "p": 50, "t" :30,"dp": 1000, "q":100, "start":"2020-02-08T07:00", "lastupdate":"2020-02-09T07:00", "quality":192},</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>3</v>
       </c>
@@ -7976,7 +7963,7 @@
         <v>{ "flid": 3,"chid":3, "p": 50, "t" :30,"dp": 1000, "q":100, "start":"2020-02-09T07:00", "lastupdate":"2020-02-10T07:00", "quality":192},</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>4</v>
       </c>
@@ -8009,7 +7996,7 @@
         <v>{ "flid": 4,"chid":4, "p": 50, "t" :30,"dp": 1000, "q":100, "start":"2020-02-01T07:00", "lastupdate":"2020-02-02T07:00", "quality":192},</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>4</v>
       </c>
@@ -8042,7 +8029,7 @@
         <v>{ "flid": 4,"chid":4, "p": 50, "t" :30,"dp": 1000, "q":100, "start":"2020-02-02T07:00", "lastupdate":"2020-02-03T07:00", "quality":192},</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>4</v>
       </c>
@@ -8075,7 +8062,7 @@
         <v>{ "flid": 4,"chid":4, "p": 50, "t" :30,"dp": 1000, "q":100, "start":"2020-02-03T07:00", "lastupdate":"2020-02-04T07:00", "quality":192},</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>4</v>
       </c>
@@ -8108,7 +8095,7 @@
         <v>{ "flid": 4,"chid":4, "p": 50, "t" :30,"dp": 1000, "q":100, "start":"2020-02-04T07:00", "lastupdate":"2020-02-05T07:00", "quality":192},</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>4</v>
       </c>
@@ -8141,7 +8128,7 @@
         <v>{ "flid": 4,"chid":4, "p": 50, "t" :30,"dp": 1000, "q":100, "start":"2020-02-05T07:00", "lastupdate":"2020-02-06T07:00", "quality":192},</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>4</v>
       </c>
@@ -8174,7 +8161,7 @@
         <v>{ "flid": 4,"chid":4, "p": 50, "t" :30,"dp": 1000, "q":100, "start":"2020-02-06T07:00", "lastupdate":"2020-02-07T07:00", "quality":192},</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>4</v>
       </c>
@@ -8207,7 +8194,7 @@
         <v>{ "flid": 4,"chid":4, "p": 50, "t" :30,"dp": 1000, "q":100, "start":"2020-02-07T07:00", "lastupdate":"2020-02-08T07:00", "quality":192},</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>4</v>
       </c>
@@ -8240,7 +8227,7 @@
         <v>{ "flid": 4,"chid":4, "p": 50, "t" :30,"dp": 1000, "q":100, "start":"2020-02-08T07:00", "lastupdate":"2020-02-09T07:00", "quality":192},</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>4</v>
       </c>
@@ -8287,24 +8274,24 @@
       <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="2.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="127.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="127.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15" x14ac:dyDescent="0.3">
       <c r="H1" s="29" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="15" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>21</v>
       </c>
@@ -8336,7 +8323,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="15" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -8369,7 +8356,7 @@
         <v>{ "flid": 1,"chid":1, "CO2": 0.2332, "N2" :0.8976,"Ro": 0.9345, "xx":0, "zz":0, "lastupdate":"2020-02-19T12:01", "quality":192},</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="15" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -8402,7 +8389,7 @@
         <v>{ "flid": 1,"chid":1, "CO2": 0.2332, "N2" :0.8976,"Ro": 0.9345, "xx":0, "zz":0, "lastupdate":"2020-02-19T12:02", "quality":193},</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="15" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -8435,7 +8422,7 @@
         <v>{ "flid": 1,"chid":1, "CO2": 0.2332, "N2" :0.8976,"Ro": 0.9345, "xx":0, "zz":0, "lastupdate":"2020-02-19T12:03", "quality":194},</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="15" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>1</v>
       </c>
@@ -8468,7 +8455,7 @@
         <v>{ "flid": 1,"chid":1, "CO2": 0.2332, "N2" :0.8976,"Ro": 0.9345, "xx":0, "zz":0, "lastupdate":"2020-02-19T12:04", "quality":195},</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="15" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>1</v>
       </c>
@@ -8501,7 +8488,7 @@
         <v>{ "flid": 1,"chid":1, "CO2": 0.2332, "N2" :0.8976,"Ro": 0.9345, "xx":0, "zz":0, "lastupdate":"2020-02-19T12:05", "quality":196},</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="15" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>1</v>
       </c>
@@ -8534,7 +8521,7 @@
         <v>{ "flid": 1,"chid":1, "CO2": 0.2332, "N2" :0.8976,"Ro": 0.9345, "xx":0, "zz":0, "lastupdate":"2020-02-19T12:06", "quality":197},</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="15" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>1</v>
       </c>
@@ -8567,7 +8554,7 @@
         <v>{ "flid": 1,"chid":1, "CO2": 0.2332, "N2" :0.8976,"Ro": 0.9345, "xx":0, "zz":0, "lastupdate":"2020-02-19T12:07", "quality":198},</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="15" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>1</v>
       </c>
@@ -8600,7 +8587,7 @@
         <v>{ "flid": 1,"chid":1, "CO2": 0.2332, "N2" :0.8976,"Ro": 0.9345, "xx":0, "zz":0, "lastupdate":"2020-02-19T12:08", "quality":199},</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="15" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>1</v>
       </c>
@@ -8633,7 +8620,7 @@
         <v>{ "flid": 1,"chid":1, "CO2": 0.2332, "N2" :0.8976,"Ro": 0.9345, "xx":0, "zz":0, "lastupdate":"2020-02-19T12:09", "quality":200},</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="15" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>2</v>
       </c>
@@ -8666,7 +8653,7 @@
         <v>{ "flid": 2,"chid":2, "CO2": 0.2332, "N2" :0.8976,"Ro": 0.9345, "xx":0, "zz":0, "lastupdate":"2020-02-19T12:10", "quality":201},</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="15" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>2</v>
       </c>
@@ -8699,7 +8686,7 @@
         <v>{ "flid": 2,"chid":2, "CO2": 0.2332, "N2" :0.8976,"Ro": 0.9345, "xx":0, "zz":0, "lastupdate":"2020-02-19T12:11", "quality":202},</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" ht="15" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>2</v>
       </c>
@@ -8732,7 +8719,7 @@
         <v>{ "flid": 2,"chid":2, "CO2": 0.2332, "N2" :0.8976,"Ro": 0.9345, "xx":0, "zz":0, "lastupdate":"2020-02-19T12:12", "quality":203},</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" ht="15" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>2</v>
       </c>
@@ -8765,7 +8752,7 @@
         <v>{ "flid": 2,"chid":2, "CO2": 0.2332, "N2" :0.8976,"Ro": 0.9345, "xx":0, "zz":0, "lastupdate":"2020-02-19T12:13", "quality":204},</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" ht="15" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>2</v>
       </c>
@@ -8798,7 +8785,7 @@
         <v>{ "flid": 2,"chid":2, "CO2": 0.2332, "N2" :0.8976,"Ro": 0.9345, "xx":0, "zz":0, "lastupdate":"2020-02-19T12:14", "quality":205},</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" ht="15" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>2</v>
       </c>
@@ -8831,7 +8818,7 @@
         <v>{ "flid": 2,"chid":2, "CO2": 0.2332, "N2" :0.8976,"Ro": 0.9345, "xx":0, "zz":0, "lastupdate":"2020-02-19T12:15", "quality":206},</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" ht="15" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>2</v>
       </c>
@@ -8864,7 +8851,7 @@
         <v>{ "flid": 2,"chid":2, "CO2": 0.2332, "N2" :0.8976,"Ro": 0.9345, "xx":0, "zz":0, "lastupdate":"2020-02-19T12:16", "quality":207},</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" ht="15" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>2</v>
       </c>
@@ -8897,7 +8884,7 @@
         <v>{ "flid": 2,"chid":2, "CO2": 0.2332, "N2" :0.8976,"Ro": 0.9345, "xx":0, "zz":0, "lastupdate":"2020-02-19T12:17", "quality":208},</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" ht="15" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>2</v>
       </c>
@@ -8930,7 +8917,7 @@
         <v>{ "flid": 2,"chid":2, "CO2": 0.2332, "N2" :0.8976,"Ro": 0.9345, "xx":0, "zz":0, "lastupdate":"2020-02-19T12:18", "quality":209},</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" ht="15" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>3</v>
       </c>
@@ -8963,7 +8950,7 @@
         <v>{ "flid": 3,"chid":3, "CO2": 0.2332, "N2" :0.8976,"Ro": 0.9345, "xx":0, "zz":0, "lastupdate":"2020-02-19T12:19", "quality":210},</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>3</v>
       </c>
@@ -8996,7 +8983,7 @@
         <v>{ "flid": 3,"chid":3, "CO2": 0.2332, "N2" :0.8976,"Ro": 0.9345, "xx":0, "zz":0, "lastupdate":"2020-02-19T12:20", "quality":211},</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>3</v>
       </c>
@@ -9029,7 +9016,7 @@
         <v>{ "flid": 3,"chid":3, "CO2": 0.2332, "N2" :0.8976,"Ro": 0.9345, "xx":0, "zz":0, "lastupdate":"2020-02-19T12:21", "quality":212},</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>3</v>
       </c>
@@ -9062,7 +9049,7 @@
         <v>{ "flid": 3,"chid":3, "CO2": 0.2332, "N2" :0.8976,"Ro": 0.9345, "xx":0, "zz":0, "lastupdate":"2020-02-19T12:22", "quality":213},</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>3</v>
       </c>
@@ -9095,7 +9082,7 @@
         <v>{ "flid": 3,"chid":3, "CO2": 0.2332, "N2" :0.8976,"Ro": 0.9345, "xx":0, "zz":0, "lastupdate":"2020-02-19T12:23", "quality":214},</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>3</v>
       </c>
@@ -9128,7 +9115,7 @@
         <v>{ "flid": 3,"chid":3, "CO2": 0.2332, "N2" :0.8976,"Ro": 0.9345, "xx":0, "zz":0, "lastupdate":"2020-02-19T12:24", "quality":215},</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>3</v>
       </c>
@@ -9161,7 +9148,7 @@
         <v>{ "flid": 3,"chid":3, "CO2": 0.2332, "N2" :0.8976,"Ro": 0.9345, "xx":0, "zz":0, "lastupdate":"2020-02-19T12:25", "quality":216},</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>3</v>
       </c>
@@ -9194,7 +9181,7 @@
         <v>{ "flid": 3,"chid":3, "CO2": 0.2332, "N2" :0.8976,"Ro": 0.9345, "xx":0, "zz":0, "lastupdate":"2020-02-19T12:26", "quality":217},</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>3</v>
       </c>
@@ -9227,7 +9214,7 @@
         <v>{ "flid": 3,"chid":3, "CO2": 0.2332, "N2" :0.8976,"Ro": 0.9345, "xx":0, "zz":0, "lastupdate":"2020-02-19T12:27", "quality":218},</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>4</v>
       </c>
@@ -9260,7 +9247,7 @@
         <v>{ "flid": 4,"chid":4, "CO2": 0.2332, "N2" :0.8976,"Ro": 0.9345, "xx":0, "zz":0, "lastupdate":"2020-02-19T12:28", "quality":219},</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>4</v>
       </c>
@@ -9293,7 +9280,7 @@
         <v>{ "flid": 4,"chid":4, "CO2": 0.2332, "N2" :0.8976,"Ro": 0.9345, "xx":0, "zz":0, "lastupdate":"2020-02-19T12:29", "quality":220},</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>4</v>
       </c>
@@ -9326,7 +9313,7 @@
         <v>{ "flid": 4,"chid":4, "CO2": 0.2332, "N2" :0.8976,"Ro": 0.9345, "xx":0, "zz":0, "lastupdate":"2020-02-19T12:30", "quality":221},</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>4</v>
       </c>
@@ -9359,7 +9346,7 @@
         <v>{ "flid": 4,"chid":4, "CO2": 0.2332, "N2" :0.8976,"Ro": 0.9345, "xx":0, "zz":0, "lastupdate":"2020-02-19T12:31", "quality":222},</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>4</v>
       </c>
@@ -9392,7 +9379,7 @@
         <v>{ "flid": 4,"chid":4, "CO2": 0.2332, "N2" :0.8976,"Ro": 0.9345, "xx":0, "zz":0, "lastupdate":"2020-02-19T12:32", "quality":223},</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>4</v>
       </c>
@@ -9425,7 +9412,7 @@
         <v>{ "flid": 4,"chid":4, "CO2": 0.2332, "N2" :0.8976,"Ro": 0.9345, "xx":0, "zz":0, "lastupdate":"2020-02-19T12:33", "quality":224},</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>4</v>
       </c>
@@ -9458,7 +9445,7 @@
         <v>{ "flid": 4,"chid":4, "CO2": 0.2332, "N2" :0.8976,"Ro": 0.9345, "xx":0, "zz":0, "lastupdate":"2020-02-19T12:34", "quality":225},</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>4</v>
       </c>
@@ -9491,7 +9478,7 @@
         <v>{ "flid": 4,"chid":4, "CO2": 0.2332, "N2" :0.8976,"Ro": 0.9345, "xx":0, "zz":0, "lastupdate":"2020-02-19T12:35", "quality":226},</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>4</v>
       </c>
@@ -9537,37 +9524,37 @@
       <selection activeCell="AD16" sqref="AD16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.88671875" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="21.28515625" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.85546875" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.28515625" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="21.33203125" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.88671875" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24.140625" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="110.7109375" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="14.85546875" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.140625" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.28515625" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="22.140625" customWidth="1"/>
-    <col min="19" max="19" width="12.42578125" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.28515625" hidden="1" customWidth="1"/>
-    <col min="24" max="27" width="10.140625" hidden="1" customWidth="1"/>
-    <col min="28" max="28" width="5.5703125" hidden="1" customWidth="1"/>
-    <col min="29" max="29" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.109375" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="110.6640625" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="14.88671875" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.109375" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.33203125" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="22.109375" customWidth="1"/>
+    <col min="19" max="19" width="12.44140625" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.33203125" hidden="1" customWidth="1"/>
+    <col min="24" max="27" width="10.109375" hidden="1" customWidth="1"/>
+    <col min="28" max="28" width="5.5546875" hidden="1" customWidth="1"/>
+    <col min="29" max="29" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:30" s="7" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>162</v>
       </c>
@@ -9651,7 +9638,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:30" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:30" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
         <v>164</v>
       </c>
@@ -9711,7 +9698,7 @@
         <v>{"systemid":1,"name":"ДПКС № 1","ip":"192.168.0.111","path":"xxx.yyy.zzz","period":30,"sensors":[</v>
       </c>
     </row>
-    <row r="3" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="15"/>
       <c r="B3" s="16"/>
       <c r="C3" s="16"/>
@@ -9783,7 +9770,7 @@
         <v>{"sensorid":1,"low":0,"name":"P in KC 32","path":"xxx.yyy.zzz","high":100,"chour":true,"hasR":true,"hasH":true},</v>
       </c>
     </row>
-    <row r="4" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="15"/>
       <c r="B4" s="16"/>
       <c r="C4" s="16"/>
@@ -9855,7 +9842,7 @@
         <v>{"sensorid":2,"low":0,"name":"P in KC 33","path":"xxx.yyy.zzz","high":100,"chour":true,"hasR":true,"hasH":true},</v>
       </c>
     </row>
-    <row r="5" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="17"/>
       <c r="B5" s="18"/>
       <c r="C5" s="18"/>
@@ -9927,7 +9914,7 @@
         <v>{"sensorid":3,"low":0,"name":"P in KC 34","path":"xxx.yyy.zzz","high":100,"chour":true,"hasR":true,"hasH":true}]},</v>
       </c>
     </row>
-    <row r="6" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="12" t="s">
         <v>164</v>
       </c>
@@ -9987,7 +9974,7 @@
         <v>{"systemid":2,"name":"ДПКС № 2","ip":"192.168.0.112","path":"xxx.yyy.zzz","period":30,"sensors":[</v>
       </c>
     </row>
-    <row r="7" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="15"/>
       <c r="B7" s="16"/>
       <c r="C7" s="16"/>
@@ -10059,7 +10046,7 @@
         <v>{"sensorid":4,"low":0,"name":"P in KC 36","path":"xxx.yyy.zzz","high":100,"chour":true,"hasR":true,"hasH":true},</v>
       </c>
     </row>
-    <row r="8" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="15"/>
       <c r="B8" s="16"/>
       <c r="C8" s="16"/>
@@ -10131,7 +10118,7 @@
         <v>{"sensorid":5,"low":0,"name":"P in KC 37","path":"xxx.yyy.zzz","high":100,"chour":true,"hasR":true,"hasH":true},</v>
       </c>
     </row>
-    <row r="9" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="17"/>
       <c r="B9" s="18"/>
       <c r="C9" s="18"/>
@@ -10216,26 +10203,26 @@
       <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7" customWidth="1"/>
-    <col min="7" max="7" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.5546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="138.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="138.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H1" s="29" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>189</v>
       </c>
@@ -10267,7 +10254,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -10300,7 +10287,7 @@
         <v>{ "paramid": 1,"sensorid":1, "value": 50, "state" :"good","stateDesc": "good", "user":"Ivan", "xxx":1000, "lastupdate":"2020-02-19T12:01", "quality":192},</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -10333,7 +10320,7 @@
         <v>{ "paramid": 1,"sensorid":1, "value": 50, "state" :"good","stateDesc": "good", "user":"Ivan", "xxx":1000, "lastupdate":"2020-02-19T12:02", "quality":192},</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -10366,7 +10353,7 @@
         <v>{ "paramid": 1,"sensorid":1, "value": 50, "state" :"good","stateDesc": "good", "user":"Ivan", "xxx":1000, "lastupdate":"2020-02-19T12:03", "quality":192},</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>1</v>
       </c>
@@ -10399,7 +10386,7 @@
         <v>{ "paramid": 1,"sensorid":1, "value": 50, "state" :"good","stateDesc": "good", "user":"Ivan", "xxx":1000, "lastupdate":"2020-02-19T12:04", "quality":192},</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>2</v>
       </c>
@@ -10432,7 +10419,7 @@
         <v>{ "paramid": 2,"sensorid":2, "value": 60, "state" :"good","stateDesc": "good", "user":"Ivan", "xxx":1000, "lastupdate":"2020-02-19T12:01", "quality":192},</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>2</v>
       </c>
@@ -10465,7 +10452,7 @@
         <v>{ "paramid": 2,"sensorid":2, "value": 60, "state" :"good","stateDesc": "good", "user":"Ivan", "xxx":1000, "lastupdate":"2020-02-19T12:02", "quality":192},</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>2</v>
       </c>
@@ -10498,7 +10485,7 @@
         <v>{ "paramid": 2,"sensorid":2, "value": 60, "state" :"good","stateDesc": "good", "user":"Ivan", "xxx":1000, "lastupdate":"2020-02-19T12:03", "quality":192},</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>2</v>
       </c>
@@ -10531,7 +10518,7 @@
         <v>{ "paramid": 2,"sensorid":2, "value": 60, "state" :"good","stateDesc": "good", "user":"Ivan", "xxx":1000, "lastupdate":"2020-02-19T12:04", "quality":192},</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>3</v>
       </c>
@@ -10564,7 +10551,7 @@
         <v>{ "paramid": 3,"sensorid":3, "value": 75, "state" :"good","stateDesc": "good", "user":"Ivan", "xxx":1000, "lastupdate":"2020-02-19T12:01", "quality":192},</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>3</v>
       </c>
@@ -10597,7 +10584,7 @@
         <v>{ "paramid": 3,"sensorid":3, "value": 75, "state" :"good","stateDesc": "good", "user":"Ivan", "xxx":1000, "lastupdate":"2020-02-19T12:02", "quality":192},</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>3</v>
       </c>
@@ -10630,7 +10617,7 @@
         <v>{ "paramid": 3,"sensorid":3, "value": 75, "state" :"good","stateDesc": "good", "user":"Ivan", "xxx":1000, "lastupdate":"2020-02-19T12:03", "quality":192},</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>3</v>
       </c>
@@ -10663,7 +10650,7 @@
         <v>{ "paramid": 3,"sensorid":3, "value": 75, "state" :"good","stateDesc": "good", "user":"Ivan", "xxx":1000, "lastupdate":"2020-02-19T12:04", "quality":192},</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>4</v>
       </c>
@@ -10696,7 +10683,7 @@
         <v>{ "paramid": 4,"sensorid":4, "value": 75, "state" :"good","stateDesc": "good", "user":"Ivan", "xxx":1000, "lastupdate":"2020-02-19T12:01", "quality":192},</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>4</v>
       </c>
@@ -10729,7 +10716,7 @@
         <v>{ "paramid": 4,"sensorid":4, "value": 75, "state" :"good","stateDesc": "good", "user":"Ivan", "xxx":1000, "lastupdate":"2020-02-19T12:02", "quality":192},</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>4</v>
       </c>
@@ -10762,7 +10749,7 @@
         <v>{ "paramid": 4,"sensorid":4, "value": 75, "state" :"good","stateDesc": "good", "user":"Ivan", "xxx":1000, "lastupdate":"2020-02-19T12:03", "quality":192},</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>4</v>
       </c>
@@ -10795,7 +10782,7 @@
         <v>{ "paramid": 4,"sensorid":4, "value": 75, "state" :"good","stateDesc": "good", "user":"Ivan", "xxx":1000, "lastupdate":"2020-02-19T12:04", "quality":192},</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>5</v>
       </c>
@@ -10828,7 +10815,7 @@
         <v>{ "paramid": 5,"sensorid":5, "value": 75, "state" :"good","stateDesc": "good", "user":"Ivan", "xxx":1000, "lastupdate":"2020-02-19T12:01", "quality":192},</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>5</v>
       </c>
@@ -10861,7 +10848,7 @@
         <v>{ "paramid": 5,"sensorid":5, "value": 75, "state" :"good","stateDesc": "good", "user":"Ivan", "xxx":1000, "lastupdate":"2020-02-19T12:02", "quality":192},</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>5</v>
       </c>
@@ -10894,7 +10881,7 @@
         <v>{ "paramid": 5,"sensorid":5, "value": 75, "state" :"good","stateDesc": "good", "user":"Ivan", "xxx":1000, "lastupdate":"2020-02-19T12:03", "quality":192},</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>5</v>
       </c>
@@ -10927,7 +10914,7 @@
         <v>{ "paramid": 5,"sensorid":5, "value": 75, "state" :"good","stateDesc": "good", "user":"Ivan", "xxx":1000, "lastupdate":"2020-02-19T12:04", "quality":192},</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>6</v>
       </c>
@@ -10960,7 +10947,7 @@
         <v>{ "paramid": 6,"sensorid":6, "value": 75, "state" :"good","stateDesc": "good", "user":"Ivan", "xxx":1000, "lastupdate":"2020-02-19T12:01", "quality":192},</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>6</v>
       </c>
@@ -10993,7 +10980,7 @@
         <v>{ "paramid": 6,"sensorid":6, "value": 75, "state" :"good","stateDesc": "good", "user":"Ivan", "xxx":1000, "lastupdate":"2020-02-19T12:02", "quality":192},</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>6</v>
       </c>
@@ -11026,7 +11013,7 @@
         <v>{ "paramid": 6,"sensorid":6, "value": 75, "state" :"good","stateDesc": "good", "user":"Ivan", "xxx":1000, "lastupdate":"2020-02-19T12:03", "quality":192},</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>6</v>
       </c>
@@ -11073,14 +11060,14 @@
       <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.5703125" customWidth="1"/>
-    <col min="4" max="4" width="42.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.5546875" customWidth="1"/>
+    <col min="4" max="4" width="42.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>189</v>
       </c>
@@ -11094,7 +11081,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -11109,7 +11096,7 @@
         <v>{ "paramid": 1,"sensorid":1, "name": "P in KC-1"},</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -11124,7 +11111,7 @@
         <v>{ "paramid": 2,"sensorid":2, "name": "P in KC-2"},</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -11139,7 +11126,7 @@
         <v>{ "paramid": 3,"sensorid":3, "name": "P in KC-3"},</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -11154,7 +11141,7 @@
         <v>{ "paramid": 4,"sensorid":4, "name": "P in KC-4"},</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -11169,7 +11156,7 @@
         <v>{ "paramid": 5,"sensorid":5, "name": "P in KC-5"},</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -11184,7 +11171,7 @@
         <v>{ "paramid": 6,"sensorid":6, "name": "P in KC-6"},</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -11199,7 +11186,7 @@
         <v>{ "paramid": 7,"sensorid":null, "name": "P in KC-7"},</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -11214,7 +11201,7 @@
         <v>{ "paramid": 8,"sensorid":null, "name": "P in KC-8"},</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -11229,7 +11216,7 @@
         <v>{ "paramid": 9,"sensorid":null, "name": "P in KC-9"},</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -11244,7 +11231,7 @@
         <v>{ "paramid": 10,"sensorid":null, "name": "P in KC-10"},</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -11259,7 +11246,7 @@
         <v>{ "paramid": 11,"sensorid":null, "name": "P in KC-11"},</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -11274,7 +11261,7 @@
         <v>{ "paramid": 12,"sensorid":null, "name": "P in KC-12"},</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -11289,7 +11276,7 @@
         <v>{ "paramid": 13,"sensorid":null, "name": "P in KC-13"},</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -11304,7 +11291,7 @@
         <v>{ "paramid": 14,"sensorid":null, "name": "P in KC-14"},</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -11319,7 +11306,7 @@
         <v>{ "paramid": 15,"sensorid":null, "name": "P in KC-15"},</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -11334,7 +11321,7 @@
         <v>{ "paramid": 16,"sensorid":null, "name": "P in KC-16"},</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -11349,7 +11336,7 @@
         <v>{ "paramid": 17,"sensorid":null, "name": "P in KC-17"},</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -11364,7 +11351,7 @@
         <v>{ "paramid": 18,"sensorid":null, "name": "P in KC-18"},</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -11379,7 +11366,7 @@
         <v>{ "paramid": 19,"sensorid":null, "name": "P in KC-19"},</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -11394,7 +11381,7 @@
         <v>{ "paramid": 20,"sensorid":null, "name": "P in KC-20"},</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -11409,7 +11396,7 @@
         <v>{ "paramid": 21,"sensorid":null, "name": "P in KC-21"},</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -11424,7 +11411,7 @@
         <v>{ "paramid": 22,"sensorid":null, "name": "P in KC-22"},</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -11439,7 +11426,7 @@
         <v>{ "paramid": 23,"sensorid":null, "name": "P in KC-23"},</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>24</v>
       </c>

</xml_diff>

<commit_message>
group pvvg by object_id
</commit_message>
<xml_diff>
--- a/xls/create-test-data.xlsx
+++ b/xls/create-test-data.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\source\node\oask-gtp-webapi\xls\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="24912" windowHeight="12840" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="120" yWindow="60" windowWidth="24915" windowHeight="12840" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Корр-каналы" sheetId="5" r:id="rId1"/>
@@ -24,12 +19,12 @@
     <sheet name="GuiTable" sheetId="13" r:id="rId10"/>
     <sheet name="Menu" sheetId="14" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1482" uniqueCount="350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1510" uniqueCount="367">
   <si>
     <t>isAbsP</t>
   </si>
@@ -724,15 +719,6 @@
     <t>off</t>
   </si>
   <si>
-    <t>ПСГ Ч-Партизани</t>
-  </si>
-  <si>
-    <t>ПСГ Солоха</t>
-  </si>
-  <si>
-    <t>ПСГ Олишівка</t>
-  </si>
-  <si>
     <t>Режим КС Бобровницька-05</t>
   </si>
   <si>
@@ -862,9 +848,6 @@
     <t>,"type":"</t>
   </si>
   <si>
-    <t>Кран 11</t>
-  </si>
-  <si>
     <t>ДКС Солоха Кран 11</t>
   </si>
   <si>
@@ -1079,12 +1062,75 @@
   </si>
   <si>
     <t>kc_olishevka_num_gpa</t>
+  </si>
+  <si>
+    <t>childs</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>ПВВГ Мрин</t>
+  </si>
+  <si>
+    <t>PvvgHourValue</t>
+  </si>
+  <si>
+    <t>pvvg_mrin</t>
+  </si>
+  <si>
+    <t>vtv_dks_red_partizanen</t>
+  </si>
+  <si>
+    <t>vtv_dks_solokha</t>
+  </si>
+  <si>
+    <t>vtv_dks_olishevka</t>
+  </si>
+  <si>
+    <t>ObjectEvent</t>
+  </si>
+  <si>
+    <t>kc_solokha_v_11</t>
+  </si>
+  <si>
+    <t>VtvPsgDayValue</t>
+  </si>
+  <si>
+    <t>stan_red_partizanen</t>
+  </si>
+  <si>
+    <t>stan_solokha</t>
+  </si>
+  <si>
+    <t>stan_olishevka</t>
+  </si>
+  <si>
+    <t>ВТВ ГРС Партизани</t>
+  </si>
+  <si>
+    <t>VtvGrsDayValue</t>
+  </si>
+  <si>
+    <t>vtv_grs_red_partizanen</t>
+  </si>
+  <si>
+    <t>[1,2,3,4]</t>
+  </si>
+  <si>
+    <t>ВТВ Мринське ВУ ПЗГ</t>
+  </si>
+  <si>
+    <t>vtv_mrin_psg</t>
+  </si>
+  <si>
+    <t>[11,12,13]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1479,7 +1525,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1514,7 +1560,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1729,40 +1775,40 @@
       <selection activeCell="S33" sqref="S33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="108.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.109375" customWidth="1"/>
-    <col min="14" max="14" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="28" max="29" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="101.88671875" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="108.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.140625" customWidth="1"/>
+    <col min="14" max="14" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="101.85546875" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="7" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:30" s="7" customFormat="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>22</v>
       </c>
@@ -1846,7 +1892,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:30" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:30" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>221</v>
       </c>
@@ -1906,7 +1952,7 @@
         <v>{"_id":1,"name":"Корректор № 1","ip":"192.168.0.111","ftpDir":"./","addr":1,"channels":[</v>
       </c>
     </row>
-    <row r="3" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:30" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="15"/>
       <c r="B3" s="16"/>
       <c r="C3" s="16"/>
@@ -1978,7 +2024,7 @@
         <v>{"_id":1,"chno":1,"name":"Line 1","template":"S001R1","isAbsP":true,"chour":true,"hasR":true,"hasH":true},</v>
       </c>
     </row>
-    <row r="4" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:30" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="15"/>
       <c r="B4" s="16"/>
       <c r="C4" s="16"/>
@@ -2050,7 +2096,7 @@
         <v>{"_id":2,"chno":2,"name":"Line 2","template":"S001R2","isAbsP":true,"chour":true,"hasR":true,"hasH":true},</v>
       </c>
     </row>
-    <row r="5" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:30" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="17"/>
       <c r="B5" s="18"/>
       <c r="C5" s="18"/>
@@ -2122,7 +2168,7 @@
         <v>{"_id":3,"chno":3,"name":"Line 3","template":"S001R3","isAbsP":true,"chour":true,"hasR":true,"hasH":true}]},</v>
       </c>
     </row>
-    <row r="6" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
         <v>221</v>
       </c>
@@ -2182,7 +2228,7 @@
         <v>{"_id":2,"name":"Корректор № 2","ip":"192.168.0.112","ftpDir":"./","addr":2,"channels":[</v>
       </c>
     </row>
-    <row r="7" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:30" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="15"/>
       <c r="B7" s="16"/>
       <c r="C7" s="16"/>
@@ -2254,7 +2300,7 @@
         <v>{"_id":4,"chno":1,"name":"Line 1","template":"S001R1","isAbsP":true,"chour":true,"hasR":true,"hasH":true},</v>
       </c>
     </row>
-    <row r="8" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:30" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="15"/>
       <c r="B8" s="16"/>
       <c r="C8" s="16"/>
@@ -2326,7 +2372,7 @@
         <v>{"_id":5,"chno":2,"name":"Line 2","template":"S001R2","isAbsP":true,"chour":true,"hasR":true,"hasH":true},</v>
       </c>
     </row>
-    <row r="9" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:30" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="17"/>
       <c r="B9" s="18"/>
       <c r="C9" s="18"/>
@@ -2398,7 +2444,7 @@
         <v>{"_id":6,"chno":3,"name":"Line 3","template":"S001R3","isAbsP":true,"chour":true,"hasR":true,"hasH":true}]},</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:30" ht="14.45" x14ac:dyDescent="0.3">
       <c r="AD10" s="6" t="s">
         <v>12</v>
       </c>
@@ -2417,32 +2463,32 @@
       <selection activeCell="X2" sqref="X2:X42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.33203125" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="23.6640625" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="23.7109375" customWidth="1"/>
     <col min="5" max="5" width="16" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="56.33203125" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="56.28515625" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="2.109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.88671875" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="20.6640625" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="13.6640625" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="12.44140625" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="6.6640625" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="13.6640625" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="2.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.85546875" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="20.7109375" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="13.7109375" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="12.42578125" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="6.7109375" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="13.7109375" hidden="1" customWidth="1"/>
     <col min="18" max="18" width="9" hidden="1" customWidth="1"/>
     <col min="19" max="22" width="0" hidden="1" customWidth="1"/>
-    <col min="23" max="23" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="96.88671875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="96.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="7" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:24" s="7" customFormat="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>190</v>
       </c>
@@ -2486,7 +2532,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:24" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:24" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>221</v>
       </c>
@@ -2528,7 +2574,7 @@
         <v>{"_id":1,"name":"Таблица ввод № 1","columns":[</v>
       </c>
     </row>
-    <row r="3" spans="1:24" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:24" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="40"/>
       <c r="B3" s="10"/>
       <c r="C3" s="10"/>
@@ -2569,7 +2615,7 @@
         <v>{"key":"time","label":"Время"},</v>
       </c>
     </row>
-    <row r="4" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="15"/>
       <c r="B4" s="16"/>
       <c r="C4" s="16"/>
@@ -2613,7 +2659,7 @@
         <v>{"key":"param1","label":"Параметр 1"},</v>
       </c>
     </row>
-    <row r="5" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="15"/>
       <c r="B5" s="16"/>
       <c r="C5" s="16"/>
@@ -2657,7 +2703,7 @@
         <v>{"key":"param2","label":"Параметр 2"},</v>
       </c>
     </row>
-    <row r="6" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="17"/>
       <c r="B6" s="18"/>
       <c r="C6" s="18"/>
@@ -2701,7 +2747,7 @@
         <v>{"key":"param3","label":"Параметр 3"}]},</v>
       </c>
     </row>
-    <row r="7" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
         <v>221</v>
       </c>
@@ -2743,7 +2789,7 @@
         <v>{"_id":2,"name":"Таблица ввод № 1","columns":[</v>
       </c>
     </row>
-    <row r="8" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="40"/>
       <c r="B8" s="10"/>
       <c r="C8" s="10"/>
@@ -2784,7 +2830,7 @@
         <v>{"key":"time","label":"Время"},</v>
       </c>
     </row>
-    <row r="9" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="15"/>
       <c r="B9" s="16"/>
       <c r="C9" s="16"/>
@@ -2828,7 +2874,7 @@
         <v>{"key":"param5","label":"Параметр 5"},</v>
       </c>
     </row>
-    <row r="10" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="15"/>
       <c r="B10" s="16"/>
       <c r="C10" s="16"/>
@@ -2872,7 +2918,7 @@
         <v>{"key":"param6","label":"Параметр 6"},</v>
       </c>
     </row>
-    <row r="11" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="17"/>
       <c r="B11" s="18"/>
       <c r="C11" s="18"/>
@@ -2916,7 +2962,7 @@
         <v>{"key":"param7","label":"Параметр 7"}]},</v>
       </c>
     </row>
-    <row r="12" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">
         <v>221</v>
       </c>
@@ -2927,7 +2973,7 @@
         <v>32</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="E12" s="13" t="s">
         <v>201</v>
@@ -2958,7 +3004,7 @@
         <v>{"_id":3,"name":"Режим Мринське ВУ ПЗГ","columns":[</v>
       </c>
     </row>
-    <row r="13" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="40"/>
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
@@ -2999,7 +3045,7 @@
         <v>{"key":"time","label":"Година"},</v>
       </c>
     </row>
-    <row r="14" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="15"/>
       <c r="B14" s="16"/>
       <c r="C14" s="16"/>
@@ -3013,13 +3059,13 @@
         <v>167</v>
       </c>
       <c r="H14" s="30" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="I14" s="8" t="s">
         <v>176</v>
       </c>
       <c r="J14" s="8" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="K14" s="8" t="s">
         <v>194</v>
@@ -3043,7 +3089,7 @@
         <v>{"key":"kc_bobrovnitska_05_p_in","label":"Рвх"},</v>
       </c>
     </row>
-    <row r="15" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="15"/>
       <c r="B15" s="16"/>
       <c r="C15" s="16"/>
@@ -3057,13 +3103,13 @@
         <v>167</v>
       </c>
       <c r="H15" s="30" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="I15" s="8" t="s">
         <v>176</v>
       </c>
       <c r="J15" s="8" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="K15" s="8" t="s">
         <v>194</v>
@@ -3087,7 +3133,7 @@
         <v>{"key":"kc_bobrovnitska_05_p_out","label":"Рвих"},</v>
       </c>
     </row>
-    <row r="16" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="17"/>
       <c r="B16" s="18"/>
       <c r="C16" s="18"/>
@@ -3101,13 +3147,13 @@
         <v>167</v>
       </c>
       <c r="H16" s="30" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="I16" s="8" t="s">
         <v>176</v>
       </c>
       <c r="J16" s="8" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="K16" s="8" t="s">
         <v>194</v>
@@ -3131,7 +3177,7 @@
         <v>{"key":"kc_bobrovnitska_05_e","label":"е"},</v>
       </c>
     </row>
-    <row r="17" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="17"/>
       <c r="B17" s="18"/>
       <c r="C17" s="18"/>
@@ -3145,13 +3191,13 @@
         <v>167</v>
       </c>
       <c r="H17" s="30" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="I17" s="8" t="s">
         <v>176</v>
       </c>
       <c r="J17" s="8" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="K17" s="8" t="s">
         <v>194</v>
@@ -3175,7 +3221,7 @@
         <v>{"key":"kc_bobrovnitska_05_num_gpa","label":"ГПА"},</v>
       </c>
     </row>
-    <row r="18" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="17"/>
       <c r="B18" s="18"/>
       <c r="C18" s="18"/>
@@ -3189,13 +3235,13 @@
         <v>167</v>
       </c>
       <c r="H18" s="30" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="I18" s="8" t="s">
         <v>176</v>
       </c>
       <c r="J18" s="8" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="K18" s="8" t="s">
         <v>194</v>
@@ -3219,7 +3265,7 @@
         <v>{"key":"psg_red_partizanen_q_in","label":"Qзак"},</v>
       </c>
     </row>
-    <row r="19" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="17"/>
       <c r="B19" s="18"/>
       <c r="C19" s="18"/>
@@ -3233,13 +3279,13 @@
         <v>167</v>
       </c>
       <c r="H19" s="30" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="I19" s="8" t="s">
         <v>176</v>
       </c>
       <c r="J19" s="8" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="K19" s="8" t="s">
         <v>194</v>
@@ -3263,7 +3309,7 @@
         <v>{"key":"psg_red_partizanen_q_out","label":"Qвід"},</v>
       </c>
     </row>
-    <row r="20" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="17"/>
       <c r="B20" s="18"/>
       <c r="C20" s="18"/>
@@ -3277,13 +3323,13 @@
         <v>167</v>
       </c>
       <c r="H20" s="30" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="I20" s="8" t="s">
         <v>176</v>
       </c>
       <c r="J20" s="8" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="K20" s="8" t="s">
         <v>194</v>
@@ -3307,7 +3353,7 @@
         <v>{"key":"psg_red_partizanen_num_lines","label":"#скв"},</v>
       </c>
     </row>
-    <row r="21" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="17"/>
       <c r="B21" s="18"/>
       <c r="C21" s="18"/>
@@ -3321,13 +3367,13 @@
         <v>167</v>
       </c>
       <c r="H21" s="30" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="I21" s="8" t="s">
         <v>176</v>
       </c>
       <c r="J21" s="8" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="K21" s="8" t="s">
         <v>194</v>
@@ -3351,7 +3397,7 @@
         <v>{"key":"kc_mrin_p_in","label":"Рвх"},</v>
       </c>
     </row>
-    <row r="22" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="17"/>
       <c r="B22" s="18"/>
       <c r="C22" s="18"/>
@@ -3365,13 +3411,13 @@
         <v>167</v>
       </c>
       <c r="H22" s="30" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="I22" s="8" t="s">
         <v>176</v>
       </c>
       <c r="J22" s="8" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="K22" s="8" t="s">
         <v>194</v>
@@ -3395,7 +3441,7 @@
         <v>{"key":"kc_mrin_p_out","label":"Рвих"},</v>
       </c>
     </row>
-    <row r="23" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="17"/>
       <c r="B23" s="18"/>
       <c r="C23" s="18"/>
@@ -3409,13 +3455,13 @@
         <v>167</v>
       </c>
       <c r="H23" s="30" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="I23" s="8" t="s">
         <v>176</v>
       </c>
       <c r="J23" s="8" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="K23" s="8" t="s">
         <v>194</v>
@@ -3439,7 +3485,7 @@
         <v>{"key":"kc_mrin_e","label":"е"},</v>
       </c>
     </row>
-    <row r="24" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="17"/>
       <c r="B24" s="18"/>
       <c r="C24" s="18"/>
@@ -3453,13 +3499,13 @@
         <v>167</v>
       </c>
       <c r="H24" s="30" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="I24" s="8" t="s">
         <v>176</v>
       </c>
       <c r="J24" s="8" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="K24" s="8" t="s">
         <v>194</v>
@@ -3483,7 +3529,7 @@
         <v>{"key":"kc_mrin_num_gpa","label":"ГПА"},</v>
       </c>
     </row>
-    <row r="25" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="17"/>
       <c r="B25" s="18"/>
       <c r="C25" s="18"/>
@@ -3497,13 +3543,13 @@
         <v>167</v>
       </c>
       <c r="H25" s="30" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="I25" s="8" t="s">
         <v>176</v>
       </c>
       <c r="J25" s="8" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="K25" s="8" t="s">
         <v>194</v>
@@ -3527,7 +3573,7 @@
         <v>{"key":"psg_solokha_q_in","label":"Qзак"},</v>
       </c>
     </row>
-    <row r="26" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="17"/>
       <c r="B26" s="18"/>
       <c r="C26" s="18"/>
@@ -3541,13 +3587,13 @@
         <v>167</v>
       </c>
       <c r="H26" s="30" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="I26" s="8" t="s">
         <v>176</v>
       </c>
       <c r="J26" s="8" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="K26" s="8" t="s">
         <v>194</v>
@@ -3571,7 +3617,7 @@
         <v>{"key":"psg_solokha_q_out","label":"Qвід"},</v>
       </c>
     </row>
-    <row r="27" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="17"/>
       <c r="B27" s="18"/>
       <c r="C27" s="18"/>
@@ -3585,13 +3631,13 @@
         <v>167</v>
       </c>
       <c r="H27" s="30" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="I27" s="8" t="s">
         <v>176</v>
       </c>
       <c r="J27" s="8" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="K27" s="8" t="s">
         <v>194</v>
@@ -3615,7 +3661,7 @@
         <v>{"key":"psg_solokha_num_lines","label":"#скв"},</v>
       </c>
     </row>
-    <row r="28" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="17"/>
       <c r="B28" s="18"/>
       <c r="C28" s="18"/>
@@ -3629,13 +3675,13 @@
         <v>167</v>
       </c>
       <c r="H28" s="30" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="I28" s="8" t="s">
         <v>176</v>
       </c>
       <c r="J28" s="8" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="K28" s="8" t="s">
         <v>194</v>
@@ -3659,7 +3705,7 @@
         <v>{"key":"kc_solokha_p_in","label":"Рвх"},</v>
       </c>
     </row>
-    <row r="29" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="17"/>
       <c r="B29" s="18"/>
       <c r="C29" s="18"/>
@@ -3673,13 +3719,13 @@
         <v>167</v>
       </c>
       <c r="H29" s="30" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="I29" s="8" t="s">
         <v>176</v>
       </c>
       <c r="J29" s="8" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="K29" s="8" t="s">
         <v>194</v>
@@ -3703,7 +3749,7 @@
         <v>{"key":"kc_solokha_p_out","label":"Рвих"},</v>
       </c>
     </row>
-    <row r="30" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="17"/>
       <c r="B30" s="18"/>
       <c r="C30" s="18"/>
@@ -3717,13 +3763,13 @@
         <v>167</v>
       </c>
       <c r="H30" s="30" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="I30" s="8" t="s">
         <v>176</v>
       </c>
       <c r="J30" s="8" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="K30" s="8" t="s">
         <v>194</v>
@@ -3747,7 +3793,7 @@
         <v>{"key":"kc_solokha_e","label":"е"},</v>
       </c>
     </row>
-    <row r="31" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="17"/>
       <c r="B31" s="18"/>
       <c r="C31" s="18"/>
@@ -3761,13 +3807,13 @@
         <v>167</v>
       </c>
       <c r="H31" s="30" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="I31" s="8" t="s">
         <v>176</v>
       </c>
       <c r="J31" s="8" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="K31" s="8" t="s">
         <v>194</v>
@@ -3791,7 +3837,7 @@
         <v>{"key":"kc_solokha_num_gpa","label":"ГПА"},</v>
       </c>
     </row>
-    <row r="32" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="17"/>
       <c r="B32" s="18"/>
       <c r="C32" s="18"/>
@@ -3805,13 +3851,13 @@
         <v>167</v>
       </c>
       <c r="H32" s="30" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="I32" s="8" t="s">
         <v>176</v>
       </c>
       <c r="J32" s="8" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="K32" s="8" t="s">
         <v>194</v>
@@ -3835,7 +3881,7 @@
         <v>{"key":"psg_olishevka_q_in","label":"Qзак"},</v>
       </c>
     </row>
-    <row r="33" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="17"/>
       <c r="B33" s="18"/>
       <c r="C33" s="18"/>
@@ -3849,13 +3895,13 @@
         <v>167</v>
       </c>
       <c r="H33" s="30" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="I33" s="8" t="s">
         <v>176</v>
       </c>
       <c r="J33" s="8" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="K33" s="8" t="s">
         <v>194</v>
@@ -3879,7 +3925,7 @@
         <v>{"key":"psg_olishevka_q_out","label":"Qвід"},</v>
       </c>
     </row>
-    <row r="34" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="17"/>
       <c r="B34" s="18"/>
       <c r="C34" s="18"/>
@@ -3893,13 +3939,13 @@
         <v>167</v>
       </c>
       <c r="H34" s="30" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="I34" s="8" t="s">
         <v>176</v>
       </c>
       <c r="J34" s="8" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="K34" s="8" t="s">
         <v>194</v>
@@ -3923,7 +3969,7 @@
         <v>{"key":"psg_olishevka_num_lines","label":"#скв"},</v>
       </c>
     </row>
-    <row r="35" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="17"/>
       <c r="B35" s="18"/>
       <c r="C35" s="18"/>
@@ -3937,13 +3983,13 @@
         <v>167</v>
       </c>
       <c r="H35" s="30" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="I35" s="8" t="s">
         <v>176</v>
       </c>
       <c r="J35" s="8" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="K35" s="8" t="s">
         <v>194</v>
@@ -3967,7 +4013,7 @@
         <v>{"key":"kc_olishevka_p_in","label":"Рвх"},</v>
       </c>
     </row>
-    <row r="36" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="17"/>
       <c r="B36" s="18"/>
       <c r="C36" s="18"/>
@@ -3981,13 +4027,13 @@
         <v>167</v>
       </c>
       <c r="H36" s="30" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="I36" s="8" t="s">
         <v>176</v>
       </c>
       <c r="J36" s="8" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="K36" s="8" t="s">
         <v>194</v>
@@ -4011,7 +4057,7 @@
         <v>{"key":"kc_olishevka_p_out","label":"Рвих"},</v>
       </c>
     </row>
-    <row r="37" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="17"/>
       <c r="B37" s="18"/>
       <c r="C37" s="18"/>
@@ -4025,13 +4071,13 @@
         <v>167</v>
       </c>
       <c r="H37" s="30" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="I37" s="8" t="s">
         <v>176</v>
       </c>
       <c r="J37" s="8" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="K37" s="8" t="s">
         <v>194</v>
@@ -4055,7 +4101,7 @@
         <v>{"key":"kc_olishevka_e","label":"е"},</v>
       </c>
     </row>
-    <row r="38" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="17"/>
       <c r="B38" s="18"/>
       <c r="C38" s="18"/>
@@ -4069,13 +4115,13 @@
         <v>167</v>
       </c>
       <c r="H38" s="30" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="I38" s="8" t="s">
         <v>176</v>
       </c>
       <c r="J38" s="8" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="K38" s="8" t="s">
         <v>194</v>
@@ -4099,7 +4145,7 @@
         <v>{"key":"kc_olishevka_num_gpa","label":"ГПА"},</v>
       </c>
     </row>
-    <row r="39" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="17"/>
       <c r="B39" s="18"/>
       <c r="C39" s="18"/>
@@ -4113,13 +4159,13 @@
         <v>167</v>
       </c>
       <c r="H39" s="30" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="I39" s="8" t="s">
         <v>176</v>
       </c>
       <c r="J39" s="8" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="K39" s="8" t="s">
         <v>194</v>
@@ -4143,7 +4189,7 @@
         <v>{"key":"q_in_total_ogsu","label":"Qзак ОГСУ"},</v>
       </c>
     </row>
-    <row r="40" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="17"/>
       <c r="B40" s="18"/>
       <c r="C40" s="18"/>
@@ -4157,13 +4203,13 @@
         <v>167</v>
       </c>
       <c r="H40" s="30" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="I40" s="8" t="s">
         <v>176</v>
       </c>
       <c r="J40" s="8" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="K40" s="8" t="s">
         <v>194</v>
@@ -4187,7 +4233,7 @@
         <v>{"key":"q_out_total_ogsu","label":"Qвід ОГСУ"},</v>
       </c>
     </row>
-    <row r="41" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="17"/>
       <c r="B41" s="18"/>
       <c r="C41" s="18"/>
@@ -4201,13 +4247,13 @@
         <v>167</v>
       </c>
       <c r="H41" s="30" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="I41" s="8" t="s">
         <v>176</v>
       </c>
       <c r="J41" s="8" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="K41" s="8" t="s">
         <v>194</v>
@@ -4231,7 +4277,7 @@
         <v>{"key":"q_in_total_vupzg","label":"Qзак ПСГ"},</v>
       </c>
     </row>
-    <row r="42" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="17"/>
       <c r="B42" s="18"/>
       <c r="C42" s="18"/>
@@ -4245,13 +4291,13 @@
         <v>167</v>
       </c>
       <c r="H42" s="30" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="I42" s="8" t="s">
         <v>176</v>
       </c>
       <c r="J42" s="8" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="K42" s="8" t="s">
         <v>194</v>
@@ -4289,22 +4335,22 @@
       <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="46.88671875" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="12.44140625" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="15.33203125" customWidth="1"/>
+    <col min="6" max="6" width="46.85546875" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" customWidth="1"/>
     <col min="9" max="9" width="16" customWidth="1"/>
-    <col min="10" max="10" width="10.109375" customWidth="1"/>
+    <col min="10" max="10" width="10.140625" customWidth="1"/>
     <col min="12" max="22" width="0" hidden="1" customWidth="1"/>
-    <col min="24" max="24" width="36.88671875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="36.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:24" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>203</v>
       </c>
@@ -4348,7 +4394,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:24" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
         <v>221</v>
       </c>
@@ -4390,7 +4436,7 @@
         <v>{"_id":1,"name":"login1","buttons":[</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="15"/>
       <c r="B3" s="16"/>
       <c r="C3" s="16"/>
@@ -4404,13 +4450,13 @@
         <v>207</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="I3" s="8" t="s">
         <v>210</v>
       </c>
       <c r="J3" s="38" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="K3" s="38" t="s">
         <v>194</v>
@@ -4434,7 +4480,7 @@
         <v>{"label":"Режим ДКС","link":"dbo/1"},</v>
       </c>
     </row>
-    <row r="4" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="15"/>
       <c r="B4" s="16"/>
       <c r="C4" s="16"/>
@@ -4448,13 +4494,13 @@
         <v>207</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="I4" s="8" t="s">
         <v>210</v>
       </c>
       <c r="J4" s="38" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="K4" s="38" t="s">
         <v>194</v>
@@ -4478,7 +4524,7 @@
         <v>{"label":"Режим ПСГ","link":"dbo/2"},</v>
       </c>
     </row>
-    <row r="5" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="17"/>
       <c r="B5" s="18"/>
       <c r="C5" s="18"/>
@@ -4492,13 +4538,13 @@
         <v>207</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="I5" s="8" t="s">
         <v>210</v>
       </c>
       <c r="J5" s="38" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="K5" s="38" t="s">
         <v>194</v>
@@ -4522,7 +4568,7 @@
         <v>{"label":"ВТВ","link":"dbo/3"}]},</v>
       </c>
     </row>
-    <row r="6" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:24" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="12" t="s">
         <v>221</v>
       </c>
@@ -4533,7 +4579,7 @@
         <v>32</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="E6" s="13" t="s">
         <v>206</v>
@@ -4564,7 +4610,7 @@
         <v>{"_id":2,"name":"login2","buttons":[</v>
       </c>
     </row>
-    <row r="7" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="15"/>
       <c r="B7" s="16"/>
       <c r="C7" s="16"/>
@@ -4578,13 +4624,13 @@
         <v>207</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="I7" s="8" t="s">
         <v>210</v>
       </c>
       <c r="J7" s="38" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="K7" s="38" t="s">
         <v>194</v>
@@ -4608,7 +4654,7 @@
         <v>{"label":"Режим ДКС","link":"dbo/5"},</v>
       </c>
     </row>
-    <row r="8" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="15"/>
       <c r="B8" s="16"/>
       <c r="C8" s="16"/>
@@ -4622,13 +4668,13 @@
         <v>207</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="I8" s="8" t="s">
         <v>210</v>
       </c>
       <c r="J8" s="38" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="K8" s="38" t="s">
         <v>194</v>
@@ -4652,7 +4698,7 @@
         <v>{"label":"Режим ПСГ","link":"dbo/6"},</v>
       </c>
     </row>
-    <row r="9" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="17"/>
       <c r="B9" s="18"/>
       <c r="C9" s="18"/>
@@ -4666,13 +4712,13 @@
         <v>207</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="I9" s="8" t="s">
         <v>210</v>
       </c>
       <c r="J9" s="38" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K9" s="38" t="s">
         <v>194</v>
@@ -4696,7 +4742,7 @@
         <v>{"label":"ВТВ","link":"dbo/7"}]},</v>
       </c>
     </row>
-    <row r="10" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:24" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="12" t="s">
         <v>221</v>
       </c>
@@ -4707,7 +4753,7 @@
         <v>32</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="E10" s="13" t="s">
         <v>206</v>
@@ -4738,7 +4784,7 @@
         <v>{"_id":3,"name":"login3","buttons":[</v>
       </c>
     </row>
-    <row r="11" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="15"/>
       <c r="B11" s="16"/>
       <c r="C11" s="16"/>
@@ -4752,13 +4798,13 @@
         <v>207</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="I11" s="8" t="s">
         <v>210</v>
       </c>
       <c r="J11" s="38" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="K11" s="38" t="s">
         <v>194</v>
@@ -4782,7 +4828,7 @@
         <v>{"label":"Режим ДКС","link":"dbo/9"},</v>
       </c>
     </row>
-    <row r="12" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="15"/>
       <c r="B12" s="16"/>
       <c r="C12" s="16"/>
@@ -4796,13 +4842,13 @@
         <v>207</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="I12" s="8" t="s">
         <v>210</v>
       </c>
       <c r="J12" s="38" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="K12" s="38" t="s">
         <v>194</v>
@@ -4826,7 +4872,7 @@
         <v>{"label":"Режим ПСГ","link":"dbo/10"},</v>
       </c>
     </row>
-    <row r="13" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="17"/>
       <c r="B13" s="18"/>
       <c r="C13" s="18"/>
@@ -4840,13 +4886,13 @@
         <v>207</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="I13" s="8" t="s">
         <v>210</v>
       </c>
       <c r="J13" s="38" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="K13" s="38" t="s">
         <v>194</v>
@@ -4870,7 +4916,7 @@
         <v>{"label":"ВТВ","link":"dbo/11"},</v>
       </c>
     </row>
-    <row r="14" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="17"/>
       <c r="B14" s="18"/>
       <c r="C14" s="18"/>
@@ -4884,13 +4930,13 @@
         <v>207</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="I14" s="8" t="s">
         <v>210</v>
       </c>
       <c r="J14" s="38" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="K14" s="38" t="s">
         <v>194</v>
@@ -4914,7 +4960,7 @@
         <v>{"label":"Стан ПСГ","link":"dbo/12"},</v>
       </c>
     </row>
-    <row r="15" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="17"/>
       <c r="B15" s="18"/>
       <c r="C15" s="18"/>
@@ -4928,13 +4974,13 @@
         <v>207</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="I15" s="8" t="s">
         <v>210</v>
       </c>
       <c r="J15" s="38" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="K15" s="38" t="s">
         <v>194</v>
@@ -4958,7 +5004,7 @@
         <v>{"label":"Стан крану","link":"dbo/13"},</v>
       </c>
     </row>
-    <row r="16" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="17"/>
       <c r="B16" s="18"/>
       <c r="C16" s="18"/>
@@ -4978,7 +5024,7 @@
         <v>210</v>
       </c>
       <c r="J16" s="38" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="K16" s="38" t="s">
         <v>194</v>
@@ -5002,7 +5048,7 @@
         <v>{"label":"Кнопка 14","link":"dbo/14"},</v>
       </c>
     </row>
-    <row r="17" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="17"/>
       <c r="B17" s="18"/>
       <c r="C17" s="18"/>
@@ -5022,7 +5068,7 @@
         <v>210</v>
       </c>
       <c r="J17" s="38" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="K17" s="38" t="s">
         <v>194</v>
@@ -5046,7 +5092,7 @@
         <v>{"label":"Кнопка 15","link":"dbo/15"},</v>
       </c>
     </row>
-    <row r="18" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="17"/>
       <c r="B18" s="18"/>
       <c r="C18" s="18"/>
@@ -5066,7 +5112,7 @@
         <v>210</v>
       </c>
       <c r="J18" s="38" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="K18" s="38" t="s">
         <v>194</v>
@@ -5090,7 +5136,7 @@
         <v>{"label":"Кнопка 16","link":"dbo/16"},</v>
       </c>
     </row>
-    <row r="19" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="17"/>
       <c r="B19" s="18"/>
       <c r="C19" s="18"/>
@@ -5110,7 +5156,7 @@
         <v>210</v>
       </c>
       <c r="J19" s="38" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="K19" s="38" t="s">
         <v>194</v>
@@ -5134,7 +5180,7 @@
         <v>{"label":"Кнопка 17","link":"dbo/17"},</v>
       </c>
     </row>
-    <row r="20" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="17"/>
       <c r="B20" s="18"/>
       <c r="C20" s="18"/>
@@ -5154,7 +5200,7 @@
         <v>210</v>
       </c>
       <c r="J20" s="38" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="K20" s="38" t="s">
         <v>194</v>
@@ -5178,7 +5224,7 @@
         <v>{"label":"Кнопка 18","link":"dbo/18"},</v>
       </c>
     </row>
-    <row r="21" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="17"/>
       <c r="B21" s="18"/>
       <c r="C21" s="18"/>
@@ -5198,7 +5244,7 @@
         <v>210</v>
       </c>
       <c r="J21" s="38" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="K21" s="38" t="s">
         <v>194</v>
@@ -5233,23 +5279,24 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A2:F19"/>
+  <dimension ref="A2:G20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="108.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="121.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
         <v>218</v>
       </c>
@@ -5257,7 +5304,7 @@
         <v>217</v>
       </c>
       <c r="C2" s="28" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="D2" s="28" t="s">
         <v>166</v>
@@ -5265,327 +5312,431 @@
       <c r="E2" s="39" t="s">
         <v>228</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="39" t="s">
+        <v>346</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="D3" s="30" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="E3" s="30">
         <v>1</v>
       </c>
-      <c r="F3" s="1" t="str">
-        <f>CONCATENATE("{ ""_id"" :",A3,", ""fullname"":""",B3,""", ""model"":""",C3,""", ""key"": """,D3,"""",",""form_id"":",E3,"},")</f>
-        <v>{ "_id" :1, "fullname":"Режим КС Бобровницька-05", "model":"DksRegim", "key": "kc_bobrovnitska_05","form_id":1},</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F3" s="30" t="s">
+        <v>347</v>
+      </c>
+      <c r="G3" s="1" t="str">
+        <f>CONCATENATE("{ ""_id"" :",A3,", ""fullname"":""",B3,""", ""model"":""",C3,""", ""key"": """,D3,"""",",""form_id"":",E3,",""childs"":",F3,"},")</f>
+        <v>{ "_id" :1, "fullname":"Режим КС Бобровницька-05", "model":"DksRegim", "key": "kc_bobrovnitska_05","form_id":1,"childs":[]},</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="D4" s="30" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="E4" s="30">
         <v>1</v>
       </c>
-      <c r="F4" s="1" t="str">
-        <f t="shared" ref="F4:F16" si="0">CONCATENATE("{ ""_id"" :",A4,", ""fullname"":""",B4,""", ""model"":""",C4,""", ""key"": """,D4,"""",",""form_id"":",E4,"},")</f>
-        <v>{ "_id" :2, "fullname":"Режим ДКС Мрин", "model":"DksRegim", "key": "kc_mrin","form_id":1},</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F4" s="30" t="s">
+        <v>347</v>
+      </c>
+      <c r="G4" s="1" t="str">
+        <f t="shared" ref="G4:G19" si="0">CONCATENATE("{ ""_id"" :",A4,", ""fullname"":""",B4,""", ""model"":""",C4,""", ""key"": """,D4,"""",",""form_id"":",E4,",""childs"":",F4,"},")</f>
+        <v>{ "_id" :2, "fullname":"Режим ДКС Мрин", "model":"DksRegim", "key": "kc_mrin","form_id":1,"childs":[]},</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="D5" s="30" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="E5" s="30">
         <v>1</v>
       </c>
-      <c r="F5" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>{ "_id" :3, "fullname":"Режим ДКС Солоха", "model":"DksRegim", "key": "kc_solokha","form_id":1},</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F5" s="30" t="s">
+        <v>347</v>
+      </c>
+      <c r="G5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "_id" :3, "fullname":"Режим ДКС Солоха", "model":"DksRegim", "key": "kc_solokha","form_id":1,"childs":[]},</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="D6" s="30" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="E6" s="30">
         <v>1</v>
       </c>
-      <c r="F6" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>{ "_id" :4, "fullname":"Режим ДКС Олишівка", "model":"DksRegim", "key": "kc_olishevka","form_id":1},</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F6" s="30" t="s">
+        <v>347</v>
+      </c>
+      <c r="G6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "_id" :4, "fullname":"Режим ДКС Олишівка", "model":"DksRegim", "key": "kc_olishevka","form_id":1,"childs":[]},</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="D7" s="30" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="E7" s="30">
         <v>2</v>
       </c>
-      <c r="F7" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>{ "_id" :5, "fullname":"Режим ПСГ Ч-Партизани", "model":"PsgRegim", "key": "psg_red_partizanen","form_id":2},</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F7" s="30" t="s">
+        <v>347</v>
+      </c>
+      <c r="G7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "_id" :5, "fullname":"Режим ПСГ Ч-Партизани", "model":"PsgRegim", "key": "psg_red_partizanen","form_id":2,"childs":[]},</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="D8" s="30" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="E8" s="30">
         <v>2</v>
       </c>
-      <c r="F8" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>{ "_id" :6, "fullname":"Режим ПСГ Солоха", "model":"PsgRegim", "key": "psg_solokha","form_id":2},</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F8" s="30" t="s">
+        <v>347</v>
+      </c>
+      <c r="G8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "_id" :6, "fullname":"Режим ПСГ Солоха", "model":"PsgRegim", "key": "psg_solokha","form_id":2,"childs":[]},</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="D9" s="30" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="E9" s="30">
         <v>2</v>
       </c>
-      <c r="F9" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>{ "_id" :7, "fullname":"Режим ПСГ Олишівка", "model":"PsgRegim", "key": "psg_olishevka","form_id":2},</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F9" s="30" t="s">
+        <v>347</v>
+      </c>
+      <c r="G9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "_id" :7, "fullname":"Режим ПСГ Олишівка", "model":"PsgRegim", "key": "psg_olishevka","form_id":2,"childs":[]},</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>231</v>
+        <v>354</v>
       </c>
       <c r="D10" s="30" t="s">
-        <v>244</v>
+        <v>357</v>
       </c>
       <c r="E10" s="30">
         <v>3</v>
       </c>
-      <c r="F10" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>{ "_id" :8, "fullname":"Стан ПСГ Ч-Партизани", "model":"ПСГ Ч-Партизани", "key": "Стан","form_id":3},</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F10" s="30" t="s">
+        <v>347</v>
+      </c>
+      <c r="G10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "_id" :8, "fullname":"Стан ПСГ Ч-Партизани", "model":"ObjectEvent", "key": "stan_red_partizanen","form_id":3,"childs":[]},</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>232</v>
+        <v>354</v>
       </c>
       <c r="D11" s="30" t="s">
-        <v>244</v>
+        <v>358</v>
       </c>
       <c r="E11" s="30">
         <v>3</v>
       </c>
-      <c r="F11" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>{ "_id" :9, "fullname":"Стан ПСГ Солоха", "model":"ПСГ Солоха", "key": "Стан","form_id":3},</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F11" s="30" t="s">
+        <v>347</v>
+      </c>
+      <c r="G11" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "_id" :9, "fullname":"Стан ПСГ Солоха", "model":"ObjectEvent", "key": "stan_solokha","form_id":3,"childs":[]},</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>233</v>
+        <v>354</v>
       </c>
       <c r="D12" s="30" t="s">
-        <v>244</v>
+        <v>359</v>
       </c>
       <c r="E12" s="30">
         <v>3</v>
       </c>
-      <c r="F12" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>{ "_id" :10, "fullname":"Стан ПСГ Олишівка", "model":"ПСГ Олишівка", "key": "Стан","form_id":3},</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F12" s="30" t="s">
+        <v>347</v>
+      </c>
+      <c r="G12" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "_id" :10, "fullname":"Стан ПСГ Олишівка", "model":"ObjectEvent", "key": "stan_olishevka","form_id":3,"childs":[]},</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>231</v>
+        <v>356</v>
       </c>
       <c r="D13" s="30" t="s">
-        <v>248</v>
+        <v>351</v>
       </c>
       <c r="E13" s="30">
         <v>4</v>
       </c>
-      <c r="F13" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>{ "_id" :11, "fullname":"ВТВ ПСГ Ч-Партизани", "model":"ПСГ Ч-Партизани", "key": "ВТВ","form_id":4},</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F13" s="30" t="s">
+        <v>347</v>
+      </c>
+      <c r="G13" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "_id" :11, "fullname":"ВТВ ПСГ Ч-Партизани", "model":"VtvPsgDayValue", "key": "vtv_dks_red_partizanen","form_id":4,"childs":[]},</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>232</v>
+        <v>356</v>
       </c>
       <c r="D14" s="30" t="s">
-        <v>248</v>
+        <v>352</v>
       </c>
       <c r="E14" s="30">
         <v>4</v>
       </c>
-      <c r="F14" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>{ "_id" :12, "fullname":"ВТВ ПСГ Солоха", "model":"ПСГ Солоха", "key": "ВТВ","form_id":4},</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F14" s="30" t="s">
+        <v>347</v>
+      </c>
+      <c r="G14" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "_id" :12, "fullname":"ВТВ ПСГ Солоха", "model":"VtvPsgDayValue", "key": "vtv_dks_solokha","form_id":4,"childs":[]},</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>233</v>
+        <v>356</v>
       </c>
       <c r="D15" s="30" t="s">
-        <v>248</v>
+        <v>353</v>
       </c>
       <c r="E15" s="30">
         <v>4</v>
       </c>
-      <c r="F15" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>{ "_id" :13, "fullname":"ВТВ ПСГ Олишівка", "model":"ПСГ Олишівка", "key": "ВТВ","form_id":4},</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F15" s="30" t="s">
+        <v>347</v>
+      </c>
+      <c r="G15" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "_id" :13, "fullname":"ВТВ ПСГ Олишівка", "model":"VtvPsgDayValue", "key": "vtv_dks_olishevka","form_id":4,"childs":[]},</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>278</v>
+        <v>364</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="D16" s="30">
-        <v>11</v>
+        <v>356</v>
+      </c>
+      <c r="D16" s="30" t="s">
+        <v>365</v>
       </c>
       <c r="E16" s="30">
+        <v>4</v>
+      </c>
+      <c r="F16" s="30" t="s">
+        <v>366</v>
+      </c>
+      <c r="G16" s="1" t="str">
+        <f t="shared" ref="G16" si="1">CONCATENATE("{ ""_id"" :",A16,", ""fullname"":""",B16,""", ""model"":""",C16,""", ""key"": """,D16,"""",",""form_id"":",E16,",""childs"":",F16,"},")</f>
+        <v>{ "_id" :14, "fullname":"ВТВ Мринське ВУ ПЗГ", "model":"VtvPsgDayValue", "key": "vtv_mrin_psg","form_id":4,"childs":[11,12,13]},</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="D17" s="30" t="s">
+        <v>355</v>
+      </c>
+      <c r="E17" s="30">
         <v>5</v>
       </c>
-      <c r="F16" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>{ "_id" :14, "fullname":"ДКС Солоха Кран 11", "model":"Кран 11", "key": "11","form_id":5},</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="1"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="30"/>
-      <c r="E18" s="30"/>
-      <c r="F18" s="1"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="30"/>
-      <c r="E19" s="30"/>
-      <c r="F19" s="1"/>
+      <c r="F17" s="30" t="s">
+        <v>347</v>
+      </c>
+      <c r="G17" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "_id" :15, "fullname":"ДКС Солоха Кран 11", "model":"ObjectEvent", "key": "kc_solokha_v_11","form_id":5,"childs":[]},</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="D18" s="30" t="s">
+        <v>350</v>
+      </c>
+      <c r="E18" s="30">
+        <v>5</v>
+      </c>
+      <c r="F18" s="30" t="s">
+        <v>363</v>
+      </c>
+      <c r="G18" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "_id" :16, "fullname":"ПВВГ Мрин", "model":"PvvgHourValue", "key": "pvvg_mrin","form_id":5,"childs":[1,2,3,4]},</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="D19" s="30" t="s">
+        <v>362</v>
+      </c>
+      <c r="E19" s="30">
+        <v>4</v>
+      </c>
+      <c r="F19" s="30" t="s">
+        <v>347</v>
+      </c>
+      <c r="G19" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "_id" :17, "fullname":"ВТВ ГРС Партизани", "model":"VtvGrsDayValue", "key": "vtv_grs_red_partizanen","form_id":4,"childs":[]},</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="30"/>
+      <c r="G20" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5601,12 +5752,12 @@
       <selection activeCell="J41" sqref="J41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="114.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="114.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
@@ -6866,19 +7017,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3:K38"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="I42" sqref="I42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="4" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="22" customWidth="1"/>
-    <col min="10" max="10" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="145.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="145.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
@@ -8160,12 +8311,12 @@
       <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="124.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="124.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
@@ -9428,16 +9579,16 @@
       <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="2.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="2.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="118.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="118.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
@@ -10681,37 +10832,37 @@
       <selection activeCell="AD2" sqref="AD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.88671875" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="21.33203125" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.88671875" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.33203125" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24.109375" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="110.6640625" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="14.88671875" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.109375" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.33203125" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="22.109375" customWidth="1"/>
-    <col min="19" max="19" width="12.44140625" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.33203125" hidden="1" customWidth="1"/>
-    <col min="24" max="27" width="10.109375" hidden="1" customWidth="1"/>
-    <col min="28" max="28" width="5.5546875" hidden="1" customWidth="1"/>
-    <col min="29" max="29" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.140625" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="110.7109375" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="14.85546875" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.140625" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.28515625" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="22.140625" customWidth="1"/>
+    <col min="19" max="19" width="12.42578125" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.28515625" hidden="1" customWidth="1"/>
+    <col min="24" max="27" width="10.140625" hidden="1" customWidth="1"/>
+    <col min="28" max="28" width="5.5703125" hidden="1" customWidth="1"/>
+    <col min="29" max="29" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="7" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:30" s="7" customFormat="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>129</v>
       </c>
@@ -10795,7 +10946,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:30" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:30" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>131</v>
       </c>
@@ -10855,7 +11006,7 @@
         <v>{"systemid":1,"name":"ДПКС № 1","ip":"192.168.0.111","path":"xxx.yyy.zzz","period":30,"sensors":[</v>
       </c>
     </row>
-    <row r="3" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:30" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="15"/>
       <c r="B3" s="16"/>
       <c r="C3" s="16"/>
@@ -10927,7 +11078,7 @@
         <v>{"sensorid":1,"low":0,"name":"P in KC 32","path":"xxx.yyy.zzz","high":100,"chour":true,"hasR":true,"hasH":true},</v>
       </c>
     </row>
-    <row r="4" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:30" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="15"/>
       <c r="B4" s="16"/>
       <c r="C4" s="16"/>
@@ -10999,7 +11150,7 @@
         <v>{"sensorid":2,"low":0,"name":"P in KC 33","path":"xxx.yyy.zzz","high":100,"chour":true,"hasR":true,"hasH":true},</v>
       </c>
     </row>
-    <row r="5" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:30" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="17"/>
       <c r="B5" s="18"/>
       <c r="C5" s="18"/>
@@ -11071,7 +11222,7 @@
         <v>{"sensorid":3,"low":0,"name":"P in KC 34","path":"xxx.yyy.zzz","high":100,"chour":true,"hasR":true,"hasH":true}]},</v>
       </c>
     </row>
-    <row r="6" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
         <v>131</v>
       </c>
@@ -11131,7 +11282,7 @@
         <v>{"systemid":2,"name":"ДПКС № 2","ip":"192.168.0.112","path":"xxx.yyy.zzz","period":30,"sensors":[</v>
       </c>
     </row>
-    <row r="7" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:30" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="15"/>
       <c r="B7" s="16"/>
       <c r="C7" s="16"/>
@@ -11203,7 +11354,7 @@
         <v>{"sensorid":4,"low":0,"name":"P in KC 36","path":"xxx.yyy.zzz","high":100,"chour":true,"hasR":true,"hasH":true},</v>
       </c>
     </row>
-    <row r="8" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:30" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="15"/>
       <c r="B8" s="16"/>
       <c r="C8" s="16"/>
@@ -11275,7 +11426,7 @@
         <v>{"sensorid":5,"low":0,"name":"P in KC 37","path":"xxx.yyy.zzz","high":100,"chour":true,"hasR":true,"hasH":true},</v>
       </c>
     </row>
-    <row r="9" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:30" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="17"/>
       <c r="B9" s="18"/>
       <c r="C9" s="18"/>
@@ -11363,18 +11514,18 @@
       <selection activeCell="J39" sqref="J39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7" customWidth="1"/>
-    <col min="7" max="7" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="138.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="138.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
@@ -12220,33 +12371,33 @@
       <selection activeCell="AA7" sqref="AA7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="58.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.6640625" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.6640625" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.6640625" customWidth="1"/>
-    <col min="14" max="14" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.6640625" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5.5546875" customWidth="1"/>
-    <col min="21" max="21" width="26.88671875" customWidth="1"/>
-    <col min="27" max="27" width="255.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="58.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.7109375" customWidth="1"/>
+    <col min="14" max="14" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.7109375" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.5703125" customWidth="1"/>
+    <col min="21" max="21" width="26.85546875" customWidth="1"/>
+    <col min="27" max="27" width="255.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="7" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:27" s="7" customFormat="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>163</v>
       </c>
@@ -12295,7 +12446,7 @@
         <v>186</v>
       </c>
       <c r="R1" s="21" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="S1" s="21"/>
       <c r="T1" s="21"/>
@@ -12311,7 +12462,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:27" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:27" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>221</v>
       </c>
@@ -12322,7 +12473,7 @@
         <v>32</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="E2" s="13" t="s">
         <v>202</v>
@@ -12356,7 +12507,7 @@
         <v>{"_id":1,"name":"Режим КС","controls":[</v>
       </c>
     </row>
-    <row r="3" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="15"/>
       <c r="B3" s="16"/>
       <c r="C3" s="16"/>
@@ -12382,7 +12533,7 @@
         <v>178</v>
       </c>
       <c r="L3" s="41" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="M3" s="8" t="s">
         <v>181</v>
@@ -12400,7 +12551,7 @@
         <v>188</v>
       </c>
       <c r="R3" s="8" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="S3" s="8" t="s">
         <v>222</v>
@@ -12423,7 +12574,7 @@
         <v>{"key":"date","label":"Дата","value":"2020-03-18","controlType":"textbox","order":1,"type":"date","options":[{}]},</v>
       </c>
     </row>
-    <row r="4" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="15"/>
       <c r="B4" s="16"/>
       <c r="C4" s="16"/>
@@ -12467,10 +12618,10 @@
         <v>188</v>
       </c>
       <c r="R4" s="8" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="S4" s="8" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="T4" s="8" t="s">
         <v>194</v>
@@ -12490,7 +12641,7 @@
         <v>{"key":"hour","label":"Година","value":"0","controlType":"dropdown","order":2,"type":"text","options":[{"key":"+00", "value":0},{"key":"+02", "value":2},{"key":"+04", "value":4},{"key":"+06", "value":6},{"key":"+08", "value":8},{"key":"+10", "value":10},{"key":"+12", "value":12},{"key":"+14", "value":14},{"key":"+00", "value":16},{"key":"+18", "value":18},{"key":"+20", "value":20},{"key":"+22", "value":22}]},</v>
       </c>
     </row>
-    <row r="5" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="17"/>
       <c r="B5" s="18"/>
       <c r="C5" s="18"/>
@@ -12504,13 +12655,13 @@
         <v>167</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="I5" s="8" t="s">
         <v>176</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="K5" s="8" t="s">
         <v>178</v>
@@ -12534,10 +12685,10 @@
         <v>188</v>
       </c>
       <c r="R5" s="8" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="S5" s="8" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="T5" s="8" t="s">
         <v>194</v>
@@ -12557,7 +12708,7 @@
         <v>{"key":"p_in","label":"Рвх КС","value":"0","controlType":"textbox","order":3,"type":"text","options":[{}]},</v>
       </c>
     </row>
-    <row r="6" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="15"/>
       <c r="B6" s="16"/>
       <c r="C6" s="16"/>
@@ -12568,13 +12719,13 @@
         <v>167</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="I6" s="8" t="s">
         <v>176</v>
       </c>
       <c r="J6" s="8" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="K6" s="8" t="s">
         <v>178</v>
@@ -12598,10 +12749,10 @@
         <v>188</v>
       </c>
       <c r="R6" s="8" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="S6" s="8" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="T6" s="8" t="s">
         <v>194</v>
@@ -12621,7 +12772,7 @@
         <v>{"key":"p_out","label":"Рвих КС","value":"0","controlType":"textbox","order":4,"type":"text","options":[{}]},</v>
       </c>
     </row>
-    <row r="7" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="15"/>
       <c r="B7" s="16"/>
       <c r="C7" s="16"/>
@@ -12632,13 +12783,13 @@
         <v>167</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="I7" s="8" t="s">
         <v>176</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="K7" s="8" t="s">
         <v>178</v>
@@ -12662,10 +12813,10 @@
         <v>188</v>
       </c>
       <c r="R7" s="8" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="S7" s="8" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="T7" s="8" t="s">
         <v>194</v>
@@ -12685,7 +12836,7 @@
         <v>{"key":"num_gpa","label":"ГПА","value":"0","controlType":"textbox","order":4,"type":"text","options":[{}]}]},</v>
       </c>
     </row>
-    <row r="8" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
         <v>221</v>
       </c>
@@ -12696,7 +12847,7 @@
         <v>32</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="E8" s="13" t="s">
         <v>202</v>
@@ -12730,7 +12881,7 @@
         <v>{"_id":2,"name":"Режим ПСГ","controls":[</v>
       </c>
     </row>
-    <row r="9" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="15"/>
       <c r="B9" s="16"/>
       <c r="C9" s="16"/>
@@ -12756,7 +12907,7 @@
         <v>178</v>
       </c>
       <c r="L9" s="41" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="M9" s="8" t="s">
         <v>181</v>
@@ -12774,7 +12925,7 @@
         <v>188</v>
       </c>
       <c r="R9" s="8" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="S9" s="8" t="s">
         <v>222</v>
@@ -12797,7 +12948,7 @@
         <v>{"key":"date","label":"Дата","value":"2020-03-18","controlType":"textbox","order":1,"type":"date","options":[{}]},</v>
       </c>
     </row>
-    <row r="10" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="15"/>
       <c r="B10" s="16"/>
       <c r="C10" s="16"/>
@@ -12841,10 +12992,10 @@
         <v>188</v>
       </c>
       <c r="R10" s="8" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="S10" s="8" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="T10" s="8" t="s">
         <v>194</v>
@@ -12864,7 +13015,7 @@
         <v>{"key":"hour","label":"Година","value":"0","controlType":"dropdown","order":2,"type":"text","options":[{"key":"+00", "value":0},{"key":"+02", "value":2},{"key":"+04", "value":4},{"key":"+06", "value":6},{"key":"+08", "value":8},{"key":"+10", "value":10},{"key":"+12", "value":12},{"key":"+14", "value":14},{"key":"+00", "value":16},{"key":"+18", "value":18},{"key":"+20", "value":20},{"key":"+22", "value":22}]},</v>
       </c>
     </row>
-    <row r="11" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="17"/>
       <c r="B11" s="18"/>
       <c r="C11" s="18"/>
@@ -12878,13 +13029,13 @@
         <v>167</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="I11" s="8" t="s">
         <v>176</v>
       </c>
       <c r="J11" s="8" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="K11" s="8" t="s">
         <v>178</v>
@@ -12908,10 +13059,10 @@
         <v>188</v>
       </c>
       <c r="R11" s="8" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="S11" s="8" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="T11" s="8" t="s">
         <v>194</v>
@@ -12931,7 +13082,7 @@
         <v>{"key":"q_in","label":"Qзак","value":"0","controlType":"textbox","order":3,"type":"text","options":[{}]},</v>
       </c>
     </row>
-    <row r="12" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="17"/>
       <c r="B12" s="18"/>
       <c r="C12" s="18"/>
@@ -12945,13 +13096,13 @@
         <v>167</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="I12" s="8" t="s">
         <v>176</v>
       </c>
       <c r="J12" s="8" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="K12" s="8" t="s">
         <v>178</v>
@@ -12975,10 +13126,10 @@
         <v>188</v>
       </c>
       <c r="R12" s="8" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="S12" s="8" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="T12" s="8" t="s">
         <v>194</v>
@@ -12998,7 +13149,7 @@
         <v>{"key":"q_out","label":"Qвідб","value":"0","controlType":"textbox","order":4,"type":"text","options":[{}]},</v>
       </c>
     </row>
-    <row r="13" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="17"/>
       <c r="B13" s="18"/>
       <c r="C13" s="18"/>
@@ -13012,13 +13163,13 @@
         <v>167</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="I13" s="8" t="s">
         <v>176</v>
       </c>
       <c r="J13" s="8" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="K13" s="8" t="s">
         <v>178</v>
@@ -13042,10 +13193,10 @@
         <v>188</v>
       </c>
       <c r="R13" s="8" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="S13" s="8" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="T13" s="8" t="s">
         <v>194</v>
@@ -13065,7 +13216,7 @@
         <v>{"key":"num_lines","label":"с.роб","value":"0","controlType":"textbox","order":5,"type":"text","options":[{}]}]},</v>
       </c>
     </row>
-    <row r="14" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="12" t="s">
         <v>221</v>
       </c>
@@ -13076,7 +13227,7 @@
         <v>32</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="E14" s="13" t="s">
         <v>202</v>
@@ -13110,7 +13261,7 @@
         <v>{"_id":3,"name":"Стан ПСГ","controls":[</v>
       </c>
     </row>
-    <row r="15" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="15"/>
       <c r="B15" s="16"/>
       <c r="C15" s="16"/>
@@ -13136,7 +13287,7 @@
         <v>178</v>
       </c>
       <c r="L15" s="41" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="M15" s="8" t="s">
         <v>181</v>
@@ -13154,7 +13305,7 @@
         <v>188</v>
       </c>
       <c r="R15" s="8" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="S15" s="8" t="s">
         <v>222</v>
@@ -13177,7 +13328,7 @@
         <v>{"key":"date","label":"Дата","value":"2020-03-18","controlType":"textbox","order":1,"type":"date","options":[{}]},</v>
       </c>
     </row>
-    <row r="16" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="15"/>
       <c r="B16" s="16"/>
       <c r="C16" s="16"/>
@@ -13203,7 +13354,7 @@
         <v>178</v>
       </c>
       <c r="L16" s="41" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="M16" s="8" t="s">
         <v>181</v>
@@ -13221,7 +13372,7 @@
         <v>188</v>
       </c>
       <c r="R16" s="8" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="S16" s="8" t="s">
         <v>219</v>
@@ -13244,7 +13395,7 @@
         <v>{"key":"hour","label":"Година","value":"12:00:00","controlType":"textbox","order":2,"type":"time","options":[{}]},</v>
       </c>
     </row>
-    <row r="17" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="17"/>
       <c r="B17" s="18"/>
       <c r="C17" s="18"/>
@@ -13264,7 +13415,7 @@
         <v>176</v>
       </c>
       <c r="J17" s="8" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="K17" s="8" t="s">
         <v>178</v>
@@ -13288,16 +13439,16 @@
         <v>188</v>
       </c>
       <c r="R17" s="8" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="S17" s="8" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="T17" s="8" t="s">
         <v>194</v>
       </c>
       <c r="U17" s="8" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="V17" s="19"/>
       <c r="W17" s="19"/>
@@ -13311,7 +13462,7 @@
         <v>{"key":"state","label":"Стан","value":"0","controlType":"dropdown","order":3,"type":"text","options":[{"key":"Відбір", "value":2},{"key":"Закачка", "value":1},{"key":"Нейтральний", "value":0}]}]},</v>
       </c>
     </row>
-    <row r="18" spans="1:27" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:27" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="12" t="s">
         <v>221</v>
       </c>
@@ -13322,7 +13473,7 @@
         <v>32</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="E18" s="13" t="s">
         <v>202</v>
@@ -13356,7 +13507,7 @@
         <v>{"_id":4,"name":"ВТВ СПГ","controls":[</v>
       </c>
     </row>
-    <row r="19" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="15"/>
       <c r="B19" s="16"/>
       <c r="C19" s="16"/>
@@ -13382,7 +13533,7 @@
         <v>178</v>
       </c>
       <c r="L19" s="41" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="M19" s="8" t="s">
         <v>181</v>
@@ -13400,7 +13551,7 @@
         <v>188</v>
       </c>
       <c r="R19" s="8" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="S19" s="8" t="s">
         <v>222</v>
@@ -13423,7 +13574,7 @@
         <v>{"key":"date","label":"Дата","value":"2020-03-18","controlType":"textbox","order":1,"type":"date","options":[{}]},</v>
       </c>
     </row>
-    <row r="20" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="17"/>
       <c r="B20" s="18"/>
       <c r="C20" s="18"/>
@@ -13437,13 +13588,13 @@
         <v>167</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="I20" s="8" t="s">
         <v>176</v>
       </c>
       <c r="J20" s="8" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="K20" s="8" t="s">
         <v>178</v>
@@ -13467,10 +13618,10 @@
         <v>188</v>
       </c>
       <c r="R20" s="8" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="S20" s="8" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="T20" s="8" t="s">
         <v>194</v>
@@ -13490,7 +13641,7 @@
         <v>{"key":"dks","label":"ДКС","value":"0","controlType":"textbox","order":2,"type":"text","options":[{}]},</v>
       </c>
     </row>
-    <row r="21" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="15"/>
       <c r="B21" s="16"/>
       <c r="C21" s="16"/>
@@ -13501,13 +13652,13 @@
         <v>167</v>
       </c>
       <c r="H21" s="8" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="I21" s="8" t="s">
         <v>176</v>
       </c>
       <c r="J21" s="8" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="K21" s="8" t="s">
         <v>178</v>
@@ -13531,10 +13682,10 @@
         <v>188</v>
       </c>
       <c r="R21" s="8" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="S21" s="8" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="T21" s="8" t="s">
         <v>194</v>
@@ -13554,7 +13705,7 @@
         <v>{"key":"fuel","label":"Паливний","value":"0","controlType":"textbox","order":3,"type":"text","options":[{}]},</v>
       </c>
     </row>
-    <row r="22" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="15"/>
       <c r="B22" s="16"/>
       <c r="C22" s="16"/>
@@ -13565,13 +13716,13 @@
         <v>167</v>
       </c>
       <c r="H22" s="8" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="I22" s="8" t="s">
         <v>176</v>
       </c>
       <c r="J22" s="8" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="K22" s="8" t="s">
         <v>178</v>
@@ -13595,10 +13746,10 @@
         <v>188</v>
       </c>
       <c r="R22" s="8" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="S22" s="8" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="T22" s="8" t="s">
         <v>194</v>
@@ -13618,7 +13769,7 @@
         <v>{"key":"psg","label":"ПСГ","value":"0","controlType":"textbox","order":4,"type":"text","options":[{}]}]},</v>
       </c>
     </row>
-    <row r="23" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="12" t="s">
         <v>221</v>
       </c>
@@ -13629,7 +13780,7 @@
         <v>32</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="E23" s="13" t="s">
         <v>202</v>
@@ -13663,7 +13814,7 @@
         <v>{"_id":5,"name":"Стан крану","controls":[</v>
       </c>
     </row>
-    <row r="24" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="15"/>
       <c r="B24" s="16"/>
       <c r="C24" s="16"/>
@@ -13689,7 +13840,7 @@
         <v>178</v>
       </c>
       <c r="L24" s="41" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="M24" s="8" t="s">
         <v>181</v>
@@ -13707,7 +13858,7 @@
         <v>188</v>
       </c>
       <c r="R24" s="8" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="S24" s="8" t="s">
         <v>222</v>
@@ -13730,7 +13881,7 @@
         <v>{"key":"date","label":"Дата","value":"2020-03-18","controlType":"textbox","order":1,"type":"date","options":[{}]},</v>
       </c>
     </row>
-    <row r="25" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="15"/>
       <c r="B25" s="16"/>
       <c r="C25" s="16"/>
@@ -13756,7 +13907,7 @@
         <v>178</v>
       </c>
       <c r="L25" s="41" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="M25" s="8" t="s">
         <v>181</v>
@@ -13774,7 +13925,7 @@
         <v>188</v>
       </c>
       <c r="R25" s="8" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="S25" s="8" t="s">
         <v>219</v>
@@ -13797,7 +13948,7 @@
         <v>{"key":"hour","label":"Година","value":"12:00:00","controlType":"textbox","order":2,"type":"time","options":[{}]},</v>
       </c>
     </row>
-    <row r="26" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="17"/>
       <c r="B26" s="18"/>
       <c r="C26" s="18"/>
@@ -13817,7 +13968,7 @@
         <v>176</v>
       </c>
       <c r="J26" s="8" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="K26" s="8" t="s">
         <v>178</v>
@@ -13841,16 +13992,16 @@
         <v>188</v>
       </c>
       <c r="R26" s="8" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="S26" s="8" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="T26" s="8" t="s">
         <v>194</v>
       </c>
       <c r="U26" s="8" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="V26" s="19"/>
       <c r="W26" s="19"/>

</xml_diff>